<commit_message>
update scrape prices database
</commit_message>
<xml_diff>
--- a/excel/exchanges_historic_series.xlsx
+++ b/excel/exchanges_historic_series.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C87264E-6E4A-4C7C-9B19-2461F0AC7083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBFBC8D-B8EE-454E-899F-DA59ADECCC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Página1" sheetId="1" r:id="rId1"/>
+    <sheet name="2024" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -47,10 +47,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="#,##0.00000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -61,6 +62,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -84,11 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -307,16 +318,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -338,15 +352,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>45490</v>
       </c>
-      <c r="B2" s="3">
-        <v>6.00265</v>
+      <c r="B2" s="2">
+        <v>5.9731800000000002</v>
       </c>
       <c r="C2">
-        <v>5.4898899999999999</v>
+        <v>5.4586899999999998</v>
       </c>
       <c r="D2">
         <v>6.0790199999999999</v>
@@ -361,15 +375,15 @@
         <v>5.49</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>45490</v>
       </c>
-      <c r="B3" s="3">
-        <v>6.00265</v>
+      <c r="B3" s="2">
+        <v>5.9967499999999996</v>
       </c>
       <c r="C3">
-        <v>5.4898899999999999</v>
+        <v>5.4864600000000001</v>
       </c>
       <c r="D3">
         <v>6.0790199999999999</v>
@@ -384,12 +398,12 @@
         <v>5.49</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>45490</v>
       </c>
-      <c r="B4" s="3">
-        <v>6.00265</v>
+      <c r="B4" s="2">
+        <v>6.0023600000000004</v>
       </c>
       <c r="C4">
         <v>5.4898899999999999</v>
@@ -405,6 +419,1212 @@
       </c>
       <c r="G4">
         <v>5.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>45583</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6.00298</v>
+      </c>
+      <c r="C5">
+        <v>5.4920900000000001</v>
+      </c>
+      <c r="D5">
+        <v>6.1162000000000001</v>
+      </c>
+      <c r="E5">
+        <v>5.6785899999999998</v>
+      </c>
+      <c r="F5">
+        <v>6.09</v>
+      </c>
+      <c r="G5">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>45583</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6.0900600000000003</v>
+      </c>
+      <c r="C6">
+        <v>5.5887500000000001</v>
+      </c>
+      <c r="D6">
+        <v>6.1162000000000001</v>
+      </c>
+      <c r="E6">
+        <v>5.6785899999999998</v>
+      </c>
+      <c r="F6">
+        <v>6.09</v>
+      </c>
+      <c r="G6">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>45583</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6.0370799999999996</v>
+      </c>
+      <c r="C7">
+        <v>5.5447100000000002</v>
+      </c>
+      <c r="D7">
+        <v>6.1162000000000001</v>
+      </c>
+      <c r="E7">
+        <v>5.6785899999999998</v>
+      </c>
+      <c r="F7">
+        <v>6.09</v>
+      </c>
+      <c r="G7">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>45584</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6.0396299999999998</v>
+      </c>
+      <c r="C8">
+        <v>5.5445000000000002</v>
+      </c>
+      <c r="D8">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E8">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F8">
+        <v>6.1</v>
+      </c>
+      <c r="G8">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>45584</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6.0720099999999997</v>
+      </c>
+      <c r="C9">
+        <v>5.5788599999999997</v>
+      </c>
+      <c r="D9">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E9">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F9">
+        <v>6.1</v>
+      </c>
+      <c r="G9">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>45584</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C10">
+        <v>5.59816</v>
+      </c>
+      <c r="D10">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E10">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F10">
+        <v>6.1</v>
+      </c>
+      <c r="G10">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>45493</v>
+      </c>
+      <c r="B11">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C11">
+        <v>5.59816</v>
+      </c>
+      <c r="D11">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E11">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F11">
+        <v>6.03</v>
+      </c>
+      <c r="G11">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>45493</v>
+      </c>
+      <c r="B12">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C12">
+        <v>5.59816</v>
+      </c>
+      <c r="D12">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E12">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F12">
+        <v>6.03</v>
+      </c>
+      <c r="G12">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>45493</v>
+      </c>
+      <c r="B13">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C13">
+        <v>5.59816</v>
+      </c>
+      <c r="D13">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E13">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F13">
+        <v>6.03</v>
+      </c>
+      <c r="G13">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>45494</v>
+      </c>
+      <c r="B14">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C14">
+        <v>5.59816</v>
+      </c>
+      <c r="D14">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E14">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F14">
+        <v>6.03</v>
+      </c>
+      <c r="G14">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>45494</v>
+      </c>
+      <c r="B15">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C15">
+        <v>5.59816</v>
+      </c>
+      <c r="D15">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E15">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F15">
+        <v>6.03</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>45494</v>
+      </c>
+      <c r="B16">
+        <v>6.0363499999999997</v>
+      </c>
+      <c r="C16">
+        <v>5.5453000000000001</v>
+      </c>
+      <c r="D16">
+        <v>6.2227699999999997</v>
+      </c>
+      <c r="E16">
+        <v>5.7110200000000004</v>
+      </c>
+      <c r="F16">
+        <v>6.06</v>
+      </c>
+      <c r="G16">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>45495</v>
+      </c>
+      <c r="B17">
+        <v>6.0609000000000002</v>
+      </c>
+      <c r="C17">
+        <v>5.5717100000000004</v>
+      </c>
+      <c r="D17">
+        <v>6.1690300000000002</v>
+      </c>
+      <c r="E17">
+        <v>5.6625100000000002</v>
+      </c>
+      <c r="F17">
+        <v>6.05</v>
+      </c>
+      <c r="G17">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>45495</v>
+      </c>
+      <c r="B18">
+        <v>6.06351</v>
+      </c>
+      <c r="C18">
+        <v>5.5692599999999999</v>
+      </c>
+      <c r="D18">
+        <v>6.0240900000000002</v>
+      </c>
+      <c r="E18">
+        <v>5.6818099999999996</v>
+      </c>
+      <c r="F18">
+        <v>6.06</v>
+      </c>
+      <c r="G18">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>45495</v>
+      </c>
+      <c r="B19">
+        <v>6.0671900000000001</v>
+      </c>
+      <c r="C19">
+        <v>5.5720900000000002</v>
+      </c>
+      <c r="D19">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E19">
+        <v>5.6818099999999996</v>
+      </c>
+      <c r="F19">
+        <v>6.11</v>
+      </c>
+      <c r="G19">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>45496</v>
+      </c>
+      <c r="B20">
+        <v>6.0692899999999996</v>
+      </c>
+      <c r="C20">
+        <v>5.5933099999999998</v>
+      </c>
+      <c r="D20">
+        <v>6.1804600000000001</v>
+      </c>
+      <c r="E20">
+        <v>5.6980000000000004</v>
+      </c>
+      <c r="F20">
+        <v>6.07</v>
+      </c>
+      <c r="G20">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>45496</v>
+      </c>
+      <c r="B21">
+        <v>6.0613000000000001</v>
+      </c>
+      <c r="C21">
+        <v>5.5861900000000002</v>
+      </c>
+      <c r="D21">
+        <v>6.18811</v>
+      </c>
+      <c r="E21">
+        <v>5.7012499999999999</v>
+      </c>
+      <c r="F21">
+        <v>6.06</v>
+      </c>
+      <c r="G21">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>45496</v>
+      </c>
+      <c r="B22">
+        <v>6.0602799999999997</v>
+      </c>
+      <c r="C22">
+        <v>5.5865600000000004</v>
+      </c>
+      <c r="D22">
+        <v>6.1996200000000004</v>
+      </c>
+      <c r="E22">
+        <v>5.6980000000000004</v>
+      </c>
+      <c r="F22">
+        <v>6.07</v>
+      </c>
+      <c r="G22">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>45497</v>
+      </c>
+      <c r="B23">
+        <v>6.1232899999999999</v>
+      </c>
+      <c r="C23">
+        <v>5.6412399999999998</v>
+      </c>
+      <c r="D23">
+        <v>6.2382999999999997</v>
+      </c>
+      <c r="E23">
+        <v>5.7471199999999998</v>
+      </c>
+      <c r="F23" s="3">
+        <v>6.12</v>
+      </c>
+      <c r="G23">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>45497</v>
+      </c>
+      <c r="B24">
+        <v>6.1300400000000002</v>
+      </c>
+      <c r="C24">
+        <v>5.6542899999999996</v>
+      </c>
+      <c r="D24">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E24">
+        <v>5.77034</v>
+      </c>
+      <c r="F24" s="3">
+        <v>6.14</v>
+      </c>
+      <c r="G24">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>45497</v>
+      </c>
+      <c r="B25">
+        <v>6.1289499999999997</v>
+      </c>
+      <c r="C25">
+        <v>5.6550500000000001</v>
+      </c>
+      <c r="D25">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E25">
+        <v>5.77034</v>
+      </c>
+      <c r="F25" s="3">
+        <v>6.08</v>
+      </c>
+      <c r="G25">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>45498</v>
+      </c>
+      <c r="B26">
+        <v>6.1245200000000004</v>
+      </c>
+      <c r="C26">
+        <v>5.6501999999999999</v>
+      </c>
+      <c r="D26">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E26">
+        <v>5.76701</v>
+      </c>
+      <c r="F26" s="3">
+        <v>6.12</v>
+      </c>
+      <c r="G26">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>45498</v>
+      </c>
+      <c r="B27">
+        <v>6.1251600000000002</v>
+      </c>
+      <c r="C27">
+        <v>5.64764</v>
+      </c>
+      <c r="D27">
+        <v>6.2538999999999998</v>
+      </c>
+      <c r="E27">
+        <v>5.7570499999999996</v>
+      </c>
+      <c r="F27" s="3">
+        <v>6.13</v>
+      </c>
+      <c r="G27" s="3">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>45498</v>
+      </c>
+      <c r="B28">
+        <v>6.1287700000000003</v>
+      </c>
+      <c r="C28">
+        <v>5.6452499999999999</v>
+      </c>
+      <c r="D28">
+        <v>6.2892999999999999</v>
+      </c>
+      <c r="E28">
+        <v>5.7570499999999996</v>
+      </c>
+      <c r="F28" s="3">
+        <v>6.14</v>
+      </c>
+      <c r="G28" s="3">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>45499</v>
+      </c>
+      <c r="B29">
+        <v>6.1281999999999996</v>
+      </c>
+      <c r="C29">
+        <v>5.6402900000000002</v>
+      </c>
+      <c r="D29">
+        <v>6.2735200000000004</v>
+      </c>
+      <c r="E29">
+        <v>5.7570499999999996</v>
+      </c>
+      <c r="F29" s="3">
+        <v>6.13</v>
+      </c>
+      <c r="G29" s="3">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>45499</v>
+      </c>
+      <c r="B30">
+        <v>6.1429999999999998</v>
+      </c>
+      <c r="C30">
+        <v>5.6578400000000002</v>
+      </c>
+      <c r="D30">
+        <v>6.2813999999999997</v>
+      </c>
+      <c r="E30">
+        <v>5.7570499999999996</v>
+      </c>
+      <c r="F30" s="3">
+        <v>6.14</v>
+      </c>
+      <c r="G30" s="3">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>45499</v>
+      </c>
+      <c r="B31">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="C31">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="D31">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E31">
+        <v>5.77034</v>
+      </c>
+      <c r="F31">
+        <v>6.13</v>
+      </c>
+      <c r="G31">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>45500</v>
+      </c>
+      <c r="B32">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="C32">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="D32">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E32">
+        <v>5.77034</v>
+      </c>
+      <c r="F32">
+        <v>6.13</v>
+      </c>
+      <c r="G32">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>45500</v>
+      </c>
+      <c r="B33">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="C33">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="D33">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E33">
+        <v>5.77034</v>
+      </c>
+      <c r="F33">
+        <v>6.13</v>
+      </c>
+      <c r="G33">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>45500</v>
+      </c>
+      <c r="B34">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="C34">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="D34">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E34">
+        <v>5.77034</v>
+      </c>
+      <c r="F34">
+        <v>6.13</v>
+      </c>
+      <c r="G34">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>45501</v>
+      </c>
+      <c r="B35">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="C35">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="D35">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E35">
+        <v>5.77034</v>
+      </c>
+      <c r="F35">
+        <v>6.13</v>
+      </c>
+      <c r="G35">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>45501</v>
+      </c>
+      <c r="B36">
+        <v>6.1428500000000001</v>
+      </c>
+      <c r="C36">
+        <v>5.65665</v>
+      </c>
+      <c r="D36">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E36">
+        <v>5.7803399999999998</v>
+      </c>
+      <c r="F36">
+        <v>6.15</v>
+      </c>
+      <c r="G36">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>45501</v>
+      </c>
+      <c r="B37">
+        <v>6.1418600000000003</v>
+      </c>
+      <c r="C37">
+        <v>5.6568100000000001</v>
+      </c>
+      <c r="D37">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E37">
+        <v>5.7803399999999998</v>
+      </c>
+      <c r="F37">
+        <v>6.13</v>
+      </c>
+      <c r="G37">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>45502</v>
+      </c>
+      <c r="B38">
+        <v>6.1089200000000003</v>
+      </c>
+      <c r="C38">
+        <v>5.6509</v>
+      </c>
+      <c r="D38">
+        <v>6.2344099999999996</v>
+      </c>
+      <c r="E38">
+        <v>5.7636799999999999</v>
+      </c>
+      <c r="F38">
+        <v>6.11</v>
+      </c>
+      <c r="G38">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>45502</v>
+      </c>
+      <c r="B39">
+        <v>6.08887</v>
+      </c>
+      <c r="C39">
+        <v>5.6242999999999999</v>
+      </c>
+      <c r="D39">
+        <v>6.2188999999999997</v>
+      </c>
+      <c r="E39">
+        <v>5.7405200000000001</v>
+      </c>
+      <c r="F39">
+        <v>6.09</v>
+      </c>
+      <c r="G39">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>45502</v>
+      </c>
+      <c r="B40">
+        <v>6.0749300000000002</v>
+      </c>
+      <c r="C40">
+        <v>5.6160800000000002</v>
+      </c>
+      <c r="D40">
+        <v>6.2892999999999999</v>
+      </c>
+      <c r="E40">
+        <v>5.7306499999999998</v>
+      </c>
+      <c r="F40">
+        <v>6.14</v>
+      </c>
+      <c r="G40">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>45503</v>
+      </c>
+      <c r="B41">
+        <v>6.1143400000000003</v>
+      </c>
+      <c r="C41">
+        <v>5.6556600000000001</v>
+      </c>
+      <c r="D41">
+        <v>6.2344099999999996</v>
+      </c>
+      <c r="E41">
+        <v>5.7636799999999999</v>
+      </c>
+      <c r="F41">
+        <v>6.11</v>
+      </c>
+      <c r="G41">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>45503</v>
+      </c>
+      <c r="B42">
+        <v>6.0705400000000003</v>
+      </c>
+      <c r="C42">
+        <v>5.6123000000000003</v>
+      </c>
+      <c r="D42">
+        <v>6.1996200000000004</v>
+      </c>
+      <c r="E42">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F42">
+        <v>6.07</v>
+      </c>
+      <c r="G42">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>45503</v>
+      </c>
+      <c r="B43">
+        <v>6.0747400000000003</v>
+      </c>
+      <c r="C43">
+        <v>5.6125499999999997</v>
+      </c>
+      <c r="D43">
+        <v>6.2305200000000003</v>
+      </c>
+      <c r="E43">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F43">
+        <v>6.08</v>
+      </c>
+      <c r="G43">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>45504</v>
+      </c>
+      <c r="B44">
+        <v>6.15245</v>
+      </c>
+      <c r="C44">
+        <v>5.6746600000000003</v>
+      </c>
+      <c r="D44">
+        <v>6.2421899999999999</v>
+      </c>
+      <c r="E44">
+        <v>5.76701</v>
+      </c>
+      <c r="F44">
+        <v>6.12</v>
+      </c>
+      <c r="G44">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>45504</v>
+      </c>
+      <c r="B45">
+        <v>6.1144100000000003</v>
+      </c>
+      <c r="C45">
+        <v>5.6479900000000001</v>
+      </c>
+      <c r="D45">
+        <v>6.2460899999999997</v>
+      </c>
+      <c r="E45">
+        <v>5.77034</v>
+      </c>
+      <c r="F45">
+        <v>6.12</v>
+      </c>
+      <c r="G45">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>45504</v>
+      </c>
+      <c r="B46">
+        <v>6.1261000000000001</v>
+      </c>
+      <c r="C46">
+        <v>5.6578999999999997</v>
+      </c>
+      <c r="D46">
+        <v>6.2266500000000002</v>
+      </c>
+      <c r="E46">
+        <v>5.7736700000000001</v>
+      </c>
+      <c r="F46">
+        <v>6.08</v>
+      </c>
+      <c r="G46">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>45505</v>
+      </c>
+      <c r="B47">
+        <v>6.0955500000000002</v>
+      </c>
+      <c r="C47">
+        <v>5.6421900000000003</v>
+      </c>
+      <c r="D47">
+        <v>6.2774599999999996</v>
+      </c>
+      <c r="E47">
+        <v>5.8139500000000002</v>
+      </c>
+      <c r="F47">
+        <v>6.15</v>
+      </c>
+      <c r="G47">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>45505</v>
+      </c>
+      <c r="B48">
+        <v>6.1876199999999999</v>
+      </c>
+      <c r="C48">
+        <v>5.7348699999999999</v>
+      </c>
+      <c r="D48">
+        <v>6.3171099999999996</v>
+      </c>
+      <c r="E48">
+        <v>5.8685400000000003</v>
+      </c>
+      <c r="F48">
+        <v>6.19</v>
+      </c>
+      <c r="G48">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>45505</v>
+      </c>
+      <c r="B49">
+        <v>6.2071300000000003</v>
+      </c>
+      <c r="C49">
+        <v>5.7524199999999999</v>
+      </c>
+      <c r="D49">
+        <v>6.25</v>
+      </c>
+      <c r="E49">
+        <v>5.8685400000000003</v>
+      </c>
+      <c r="F49">
+        <v>6.1</v>
+      </c>
+      <c r="G49">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>45506</v>
+      </c>
+      <c r="B50">
+        <v>6.2333999999999996</v>
+      </c>
+      <c r="C50">
+        <v>5.7158499999999997</v>
+      </c>
+      <c r="D50">
+        <v>6.3734799999999998</v>
+      </c>
+      <c r="E50">
+        <v>5.8377100000000004</v>
+      </c>
+      <c r="F50">
+        <v>6.24</v>
+      </c>
+      <c r="G50">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>45506</v>
+      </c>
+      <c r="B51">
+        <v>6.23088</v>
+      </c>
+      <c r="C51">
+        <v>5.7095900000000004</v>
+      </c>
+      <c r="D51">
+        <v>6.25</v>
+      </c>
+      <c r="E51">
+        <v>5.8685400000000003</v>
+      </c>
+      <c r="F51">
+        <v>6.23</v>
+      </c>
+      <c r="G51">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>45506</v>
+      </c>
+      <c r="B52">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="C52">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="D52">
+        <v>6.3613200000000001</v>
+      </c>
+      <c r="E52">
+        <v>5.8445299999999998</v>
+      </c>
+      <c r="F52">
+        <v>6.23</v>
+      </c>
+      <c r="G52">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>45507</v>
+      </c>
+      <c r="B53">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="C53">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="D53">
+        <v>6.3613200000000001</v>
+      </c>
+      <c r="E53">
+        <v>5.8445299999999998</v>
+      </c>
+      <c r="F53">
+        <v>6.23</v>
+      </c>
+      <c r="G53">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>45507</v>
+      </c>
+      <c r="B54">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="C54">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="D54">
+        <v>6.3613200000000001</v>
+      </c>
+      <c r="E54">
+        <v>5.8445299999999998</v>
+      </c>
+      <c r="F54">
+        <v>6.25</v>
+      </c>
+      <c r="G54">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>45507</v>
+      </c>
+      <c r="B55">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="C55">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="D55">
+        <v>6.3613200000000001</v>
+      </c>
+      <c r="E55">
+        <v>5.8445299999999998</v>
+      </c>
+      <c r="F55">
+        <v>6.25</v>
+      </c>
+      <c r="G55">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>45508</v>
+      </c>
+      <c r="B56">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="C56">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="D56">
+        <v>6.3613200000000001</v>
+      </c>
+      <c r="E56">
+        <v>5.8445299999999998</v>
+      </c>
+      <c r="F56">
+        <v>6.25</v>
+      </c>
+      <c r="G56">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>45508</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>45508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates exchanges data base
</commit_message>
<xml_diff>
--- a/excel/exchanges_historic_series.xlsx
+++ b/excel/exchanges_historic_series.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F5AE0A-5891-4818-8021-9BE02F468D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C76141-7D05-4ADF-8386-76070E29F1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>nomadUSD</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -318,10 +321,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1801,6 +1804,351 @@
         <v>5.66</v>
       </c>
     </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
+        <v>45511</v>
+      </c>
+      <c r="B65">
+        <v>6.1179699999999997</v>
+      </c>
+      <c r="C65">
+        <v>5.6033099999999996</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65">
+        <v>6.12</v>
+      </c>
+      <c r="G65">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>45511</v>
+      </c>
+      <c r="B66">
+        <v>6.1429999999999998</v>
+      </c>
+      <c r="C66">
+        <v>5.6236600000000001</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66">
+        <v>6.15</v>
+      </c>
+      <c r="G66">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
+        <v>45511</v>
+      </c>
+      <c r="B67">
+        <v>6.1602499999999996</v>
+      </c>
+      <c r="C67">
+        <v>5.6373899999999999</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67">
+        <v>6.17</v>
+      </c>
+      <c r="G67">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>45512</v>
+      </c>
+      <c r="B68">
+        <v>6.1177400000000004</v>
+      </c>
+      <c r="C68">
+        <v>5.617</v>
+      </c>
+      <c r="D68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68">
+        <v>6.12</v>
+      </c>
+      <c r="G68">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
+        <v>45512</v>
+      </c>
+      <c r="B69">
+        <v>6.0851300000000004</v>
+      </c>
+      <c r="C69">
+        <v>5.5742599999999998</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69">
+        <v>6.09</v>
+      </c>
+      <c r="G69">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
+        <v>45512</v>
+      </c>
+      <c r="B70">
+        <v>6.0570500000000003</v>
+      </c>
+      <c r="C70">
+        <v>5.5475099999999999</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70">
+        <v>6.06</v>
+      </c>
+      <c r="G70">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>45513</v>
+      </c>
+      <c r="B71">
+        <v>6.0171000000000001</v>
+      </c>
+      <c r="C71">
+        <v>5.5172400000000001</v>
+      </c>
+      <c r="D71" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71">
+        <v>6.02</v>
+      </c>
+      <c r="G71">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
+        <v>45513</v>
+      </c>
+      <c r="B72">
+        <v>6.0211600000000001</v>
+      </c>
+      <c r="C72">
+        <v>5.5146600000000001</v>
+      </c>
+      <c r="D72" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72">
+        <v>6.03</v>
+      </c>
+      <c r="G72">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="5">
+        <v>45513</v>
+      </c>
+      <c r="B73">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="C73">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="D73">
+        <v>6.14628</v>
+      </c>
+      <c r="E73">
+        <v>5.6179699999999997</v>
+      </c>
+      <c r="F73">
+        <v>6.03</v>
+      </c>
+      <c r="G73">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>45514</v>
+      </c>
+      <c r="B74">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="C74">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="D74">
+        <v>6.14628</v>
+      </c>
+      <c r="E74">
+        <v>5.6179699999999997</v>
+      </c>
+      <c r="F74">
+        <v>6.03</v>
+      </c>
+      <c r="G74">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="5">
+        <v>45514</v>
+      </c>
+      <c r="B75">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="C75">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="D75">
+        <v>6.14628</v>
+      </c>
+      <c r="E75">
+        <v>5.6179699999999997</v>
+      </c>
+      <c r="F75">
+        <v>6.02</v>
+      </c>
+      <c r="G75">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="5">
+        <v>45514</v>
+      </c>
+      <c r="B76">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="C76">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="D76">
+        <v>6.14628</v>
+      </c>
+      <c r="E76">
+        <v>5.6179699999999997</v>
+      </c>
+      <c r="F76">
+        <v>6.02</v>
+      </c>
+      <c r="G76">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="5">
+        <v>45515</v>
+      </c>
+      <c r="B77">
+        <v>6.0078100000000001</v>
+      </c>
+      <c r="C77">
+        <v>5.4993999999999996</v>
+      </c>
+      <c r="D77">
+        <v>6.1425000000000001</v>
+      </c>
+      <c r="E77">
+        <v>5.62113</v>
+      </c>
+      <c r="F77">
+        <v>6.02</v>
+      </c>
+      <c r="G77">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="5">
+        <v>45515</v>
+      </c>
+      <c r="B78">
+        <v>6.0093300000000003</v>
+      </c>
+      <c r="C78">
+        <v>5.4977400000000003</v>
+      </c>
+      <c r="D78">
+        <v>6.1349600000000004</v>
+      </c>
+      <c r="E78">
+        <v>5.6053800000000003</v>
+      </c>
+      <c r="F78">
+        <v>6.01</v>
+      </c>
+      <c r="G78">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="5">
+        <v>45515</v>
+      </c>
+      <c r="B79">
+        <v>6.0075200000000004</v>
+      </c>
+      <c r="C79">
+        <v>5.4938399999999996</v>
+      </c>
+      <c r="D79">
+        <v>6.1652199999999997</v>
+      </c>
+      <c r="E79">
+        <v>5.6053800000000003</v>
+      </c>
+      <c r="F79">
+        <v>6.02</v>
+      </c>
+      <c r="G79">
+        <v>5.49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
extends data and add new inputs
</commit_message>
<xml_diff>
--- a/excel/exchanges_historic_series.xlsx
+++ b/excel/exchanges_historic_series.xlsx
@@ -8,19 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2412F500-5590-463C-B4D5-13CB3EF00CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0483FA8E-55F0-44A6-9E83-BE3FCAB86596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="1" r:id="rId1"/>
+    <sheet name="2024_wise_usd" sheetId="2" r:id="rId2"/>
+    <sheet name="2024_wise_eur" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2024_wise_eur'!$A$1:$D$48</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -57,14 +75,24 @@
   <si>
     <t>closing</t>
   </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -108,13 +136,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,10 +362,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J115" sqref="J115"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3390,9 +3419,3163 @@
       <c r="A118" s="5">
         <v>45528</v>
       </c>
+      <c r="B118">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="C118">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="D118">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E118">
+        <v>5.5991</v>
+      </c>
+      <c r="F118">
+        <v>6.21</v>
+      </c>
+      <c r="G118">
+        <v>5.54</v>
+      </c>
       <c r="H118" s="3" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="5">
+        <v>45529</v>
+      </c>
+      <c r="B119">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="C119">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="D119">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E119">
+        <v>5.5991</v>
+      </c>
+      <c r="F119">
+        <v>6.21</v>
+      </c>
+      <c r="G119">
+        <v>5.54</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="5">
+        <v>45529</v>
+      </c>
+      <c r="B120">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="C120">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="D120">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E120">
+        <v>5.5991</v>
+      </c>
+      <c r="F120">
+        <v>6.21</v>
+      </c>
+      <c r="G120">
+        <v>5.54</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="5">
+        <v>45529</v>
+      </c>
+      <c r="B121">
+        <v>6.1395999999999997</v>
+      </c>
+      <c r="C121">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="D121">
+        <v>6.2578199999999997</v>
+      </c>
+      <c r="E121">
+        <v>5.5991</v>
+      </c>
+      <c r="F121">
+        <v>6.21</v>
+      </c>
+      <c r="G121">
+        <v>5.54</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="5">
+        <v>45530</v>
+      </c>
+      <c r="B122">
+        <v>6.1208999999999998</v>
+      </c>
+      <c r="C122">
+        <v>5.4848999999999997</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="5">
+        <v>45530</v>
+      </c>
+      <c r="B123">
+        <v>6.1284999999999998</v>
+      </c>
+      <c r="C123">
+        <v>5.4917999999999996</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="5">
+        <v>45530</v>
+      </c>
+      <c r="B124">
+        <v>6.1401000000000003</v>
+      </c>
+      <c r="C124">
+        <v>5.4972000000000003</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G124">
+        <v>5.52</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="5">
+        <v>45531</v>
+      </c>
+      <c r="B125">
+        <v>6.1345000000000001</v>
+      </c>
+      <c r="C125">
+        <v>5.4927000000000001</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="5">
+        <v>45531</v>
+      </c>
+      <c r="B126">
+        <v>6.1538000000000004</v>
+      </c>
+      <c r="C126">
+        <v>5.5025000000000004</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="5">
+        <v>45531</v>
+      </c>
+      <c r="B127">
+        <v>6.1562000000000001</v>
+      </c>
+      <c r="C127">
+        <v>5.5094000000000003</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G127">
+        <v>5.51</v>
+      </c>
+      <c r="H127" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="5">
+        <v>45532</v>
+      </c>
+      <c r="B128">
+        <v>6.1444999999999999</v>
+      </c>
+      <c r="C128">
+        <v>5.5304000000000002</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="5">
+        <v>45532</v>
+      </c>
+      <c r="B129">
+        <v>6.1733000000000002</v>
+      </c>
+      <c r="C129">
+        <v>5.5549799999999996</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="5">
+        <v>45532</v>
+      </c>
+      <c r="B130">
+        <v>6.1912000000000003</v>
+      </c>
+      <c r="C130">
+        <v>5.5633999999999997</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G130">
+        <v>5.57</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="5">
+        <v>45533</v>
+      </c>
+      <c r="B131">
+        <v>6.2511999999999999</v>
+      </c>
+      <c r="C131">
+        <v>5.6406000000000001</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H131" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="5">
+        <v>45533</v>
+      </c>
+      <c r="B132">
+        <v>6.2274000000000003</v>
+      </c>
+      <c r="C132">
+        <v>5.6227</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="5">
+        <v>45533</v>
+      </c>
+      <c r="B133">
+        <v>6.2314999999999996</v>
+      </c>
+      <c r="C133">
+        <v>5.6288999999999998</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G133">
+        <v>5.63</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="5">
+        <v>45534</v>
+      </c>
+      <c r="B134">
+        <v>6.2614000000000001</v>
+      </c>
+      <c r="C134">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="5">
+        <v>45534</v>
+      </c>
+      <c r="B135">
+        <v>6.2282000000000002</v>
+      </c>
+      <c r="C135">
+        <v>5.6341000000000001</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="5">
+        <v>45534</v>
+      </c>
+      <c r="B136">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C136">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D136">
+        <v>6.3816199999999998</v>
+      </c>
+      <c r="E136">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F136">
+        <v>6.26</v>
+      </c>
+      <c r="G136">
+        <v>5.61</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="5">
+        <v>45535</v>
+      </c>
+      <c r="B137">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C137">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D137">
+        <v>6.3816199999999998</v>
+      </c>
+      <c r="E137">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F137">
+        <v>6.26</v>
+      </c>
+      <c r="G137">
+        <v>5.61</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="5">
+        <v>45535</v>
+      </c>
+      <c r="B138">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C138">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D138">
+        <v>6.3816199999999998</v>
+      </c>
+      <c r="E138">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F138">
+        <v>6.26</v>
+      </c>
+      <c r="G138">
+        <v>5.61</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="5">
+        <v>45535</v>
+      </c>
+      <c r="B139">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C139">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D139">
+        <v>6.3816199999999998</v>
+      </c>
+      <c r="E139">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F139">
+        <v>6.26</v>
+      </c>
+      <c r="G139">
+        <v>5.61</v>
+      </c>
+      <c r="H139" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="5">
+        <v>45536</v>
+      </c>
+      <c r="B140">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C140">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D140">
+        <v>6.3816199999999998</v>
+      </c>
+      <c r="E140">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F140">
+        <v>6.26</v>
+      </c>
+      <c r="G140">
+        <v>5.61</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="5">
+        <v>45536</v>
+      </c>
+      <c r="B141">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C141">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D141">
+        <v>6.3816199999999998</v>
+      </c>
+      <c r="E141">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F141">
+        <v>6.26</v>
+      </c>
+      <c r="G141">
+        <v>5.61</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="5">
+        <v>45536</v>
+      </c>
+      <c r="B142">
+        <v>6.2034399999999996</v>
+      </c>
+      <c r="C142">
+        <v>5.6116900000000003</v>
+      </c>
+      <c r="D142">
+        <v>6.3856900000000003</v>
+      </c>
+      <c r="E142">
+        <v>5.7240900000000003</v>
+      </c>
+      <c r="F142">
+        <v>6.26</v>
+      </c>
+      <c r="G142">
+        <v>5.61</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47E47A6-69F4-4AEB-9879-64F1134C7037}">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>45490</v>
+      </c>
+      <c r="B2">
+        <v>5.4586899999999998</v>
+      </c>
+      <c r="C2">
+        <v>5.4864600000000001</v>
+      </c>
+      <c r="D2">
+        <v>5.4898899999999999</v>
+      </c>
+      <c r="E2">
+        <f>LARGE(B2:D2,1)</f>
+        <v>5.4898899999999999</v>
+      </c>
+      <c r="F2">
+        <f>SMALL(B2:D2,1)</f>
+        <v>5.4586899999999998</v>
+      </c>
+      <c r="G2" s="6">
+        <f>AVERAGE(B2:D2)</f>
+        <v>5.4783466666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>45583</v>
+      </c>
+      <c r="B3">
+        <v>5.4920900000000001</v>
+      </c>
+      <c r="C3">
+        <v>5.5887500000000001</v>
+      </c>
+      <c r="D3">
+        <v>5.5447100000000002</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E48" si="0">LARGE(B3:D3,1)</f>
+        <v>5.5887500000000001</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F48" si="1">SMALL(B3:D3,1)</f>
+        <v>5.4920900000000001</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G48" si="2">AVERAGE(B3:D3)</f>
+        <v>5.5418500000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>45584</v>
+      </c>
+      <c r="B4">
+        <v>5.5445000000000002</v>
+      </c>
+      <c r="C4">
+        <v>5.5788599999999997</v>
+      </c>
+      <c r="D4">
+        <v>5.59816</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>5.59816</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>5.5445000000000002</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5738399999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>45493</v>
+      </c>
+      <c r="B5">
+        <v>5.59816</v>
+      </c>
+      <c r="C5">
+        <v>5.59816</v>
+      </c>
+      <c r="D5">
+        <v>5.59816</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.59816</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5.59816</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="2"/>
+        <v>5.59816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>45494</v>
+      </c>
+      <c r="B6">
+        <v>5.59816</v>
+      </c>
+      <c r="C6">
+        <v>5.59816</v>
+      </c>
+      <c r="D6">
+        <v>5.5453000000000001</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>5.59816</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>5.5453000000000001</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5805400000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>45495</v>
+      </c>
+      <c r="B7">
+        <v>5.5717100000000004</v>
+      </c>
+      <c r="C7">
+        <v>5.5692599999999999</v>
+      </c>
+      <c r="D7">
+        <v>5.5720900000000002</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>5.5720900000000002</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>5.5692599999999999</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5710199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>45496</v>
+      </c>
+      <c r="B8">
+        <v>5.5933099999999998</v>
+      </c>
+      <c r="C8">
+        <v>5.5861900000000002</v>
+      </c>
+      <c r="D8">
+        <v>5.5865600000000004</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>5.5933099999999998</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>5.5861900000000002</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5886866666666677</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>45497</v>
+      </c>
+      <c r="B9">
+        <v>5.6412399999999998</v>
+      </c>
+      <c r="C9">
+        <v>5.6542899999999996</v>
+      </c>
+      <c r="D9">
+        <v>5.6550500000000001</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>5.6550500000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>5.6412399999999998</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6501933333333332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>45498</v>
+      </c>
+      <c r="B10">
+        <v>5.6501999999999999</v>
+      </c>
+      <c r="C10">
+        <v>5.64764</v>
+      </c>
+      <c r="D10">
+        <v>5.6452499999999999</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>5.6501999999999999</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>5.6452499999999999</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6476966666666675</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>45499</v>
+      </c>
+      <c r="B11">
+        <v>5.6402900000000002</v>
+      </c>
+      <c r="C11">
+        <v>5.6578400000000002</v>
+      </c>
+      <c r="D11">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>5.6578400000000002</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>5.6402900000000002</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6514766666666674</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>45500</v>
+      </c>
+      <c r="B12">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="C12">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="D12">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="2"/>
+        <v>5.656299999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>45501</v>
+      </c>
+      <c r="B13">
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="C13">
+        <v>5.65665</v>
+      </c>
+      <c r="D13">
+        <v>5.6568100000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>5.6568100000000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>5.6562999999999999</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6565866666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>45502</v>
+      </c>
+      <c r="B14">
+        <v>5.6509</v>
+      </c>
+      <c r="C14">
+        <v>5.6242999999999999</v>
+      </c>
+      <c r="D14">
+        <v>5.6160800000000002</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>5.6509</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>5.6160800000000002</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6304266666666676</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>45503</v>
+      </c>
+      <c r="B15">
+        <v>5.6556600000000001</v>
+      </c>
+      <c r="C15">
+        <v>5.6123000000000003</v>
+      </c>
+      <c r="D15">
+        <v>5.6125499999999997</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>5.6556600000000001</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>5.6123000000000003</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6268366666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>45504</v>
+      </c>
+      <c r="B16">
+        <v>5.6746600000000003</v>
+      </c>
+      <c r="C16">
+        <v>5.6479900000000001</v>
+      </c>
+      <c r="D16">
+        <v>5.6578999999999997</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>5.6746600000000003</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>5.6479900000000001</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6601833333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>45505</v>
+      </c>
+      <c r="B17">
+        <v>5.6421900000000003</v>
+      </c>
+      <c r="C17">
+        <v>5.7348699999999999</v>
+      </c>
+      <c r="D17">
+        <v>5.7524199999999999</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>5.7524199999999999</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>5.6421900000000003</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7098266666666673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>45506</v>
+      </c>
+      <c r="B18">
+        <v>5.7158499999999997</v>
+      </c>
+      <c r="C18">
+        <v>5.7095900000000004</v>
+      </c>
+      <c r="D18">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>5.7095900000000004</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7178366666666669</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>45507</v>
+      </c>
+      <c r="B19">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="C19">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="D19">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7280699999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>45508</v>
+      </c>
+      <c r="B20">
+        <v>5.7280699999999998</v>
+      </c>
+      <c r="C20">
+        <v>5.7272100000000004</v>
+      </c>
+      <c r="D20">
+        <v>5.7281000000000004</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>5.7281000000000004</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>5.7272100000000004</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7277933333333335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>45509</v>
+      </c>
+      <c r="B21">
+        <v>5.8010999999999999</v>
+      </c>
+      <c r="C21">
+        <v>5.7407599999999999</v>
+      </c>
+      <c r="D21">
+        <v>5.7229799999999997</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>5.8010999999999999</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>5.7229799999999997</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7549466666666662</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>45510</v>
+      </c>
+      <c r="B22">
+        <v>5.6627099999999997</v>
+      </c>
+      <c r="C22">
+        <v>5.6586100000000004</v>
+      </c>
+      <c r="D22">
+        <v>5.6571600000000002</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>5.6627099999999997</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>5.6571600000000002</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6594933333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>45511</v>
+      </c>
+      <c r="B23">
+        <v>5.6033099999999996</v>
+      </c>
+      <c r="C23">
+        <v>5.6236600000000001</v>
+      </c>
+      <c r="D23">
+        <v>5.6373899999999999</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>5.6373899999999999</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>5.6033099999999996</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6214533333333323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>45512</v>
+      </c>
+      <c r="B24">
+        <v>5.617</v>
+      </c>
+      <c r="C24">
+        <v>5.5742599999999998</v>
+      </c>
+      <c r="D24">
+        <v>5.5475099999999999</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>5.617</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>5.5475099999999999</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5795899999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>45513</v>
+      </c>
+      <c r="B25">
+        <v>5.5172400000000001</v>
+      </c>
+      <c r="C25">
+        <v>5.5146600000000001</v>
+      </c>
+      <c r="D25">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>5.5172400000000001</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5135333333333341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>45514</v>
+      </c>
+      <c r="B26">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="C26">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="D26">
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>5.5087000000000002</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5087000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>45515</v>
+      </c>
+      <c r="B27">
+        <v>5.4993999999999996</v>
+      </c>
+      <c r="C27">
+        <v>5.4977400000000003</v>
+      </c>
+      <c r="D27">
+        <v>5.4938399999999996</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>5.4993999999999996</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>5.4938399999999996</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4969933333333332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>45516</v>
+      </c>
+      <c r="B28">
+        <v>5.4993999999999996</v>
+      </c>
+      <c r="C28">
+        <v>5.4877399999999996</v>
+      </c>
+      <c r="D28">
+        <v>5.4938399999999996</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>5.4993999999999996</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>5.4877399999999996</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4936599999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>45517</v>
+      </c>
+      <c r="B29">
+        <v>5.4891100000000002</v>
+      </c>
+      <c r="C29">
+        <v>5.4487899999999998</v>
+      </c>
+      <c r="D29">
+        <v>5.4572900000000004</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>5.4891100000000002</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>5.4487899999999998</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4650633333333332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>45518</v>
+      </c>
+      <c r="B30">
+        <v>5.44909</v>
+      </c>
+      <c r="C30">
+        <v>5.46896</v>
+      </c>
+      <c r="D30">
+        <v>5.4706099999999998</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>5.4706099999999998</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>5.44909</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4628866666666669</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>45519</v>
+      </c>
+      <c r="B31">
+        <v>5.4555100000000003</v>
+      </c>
+      <c r="C31">
+        <v>5.4836900000000002</v>
+      </c>
+      <c r="D31">
+        <v>5.4863400000000002</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>5.4863400000000002</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>5.4555100000000003</v>
+      </c>
+      <c r="G31" s="6">
+        <f t="shared" si="2"/>
+        <v>5.475179999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>45520</v>
+      </c>
+      <c r="B32">
+        <v>5.4542599999999997</v>
+      </c>
+      <c r="C32">
+        <v>5.46624</v>
+      </c>
+      <c r="D32">
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>5.4542599999999997</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4640133333333338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>45521</v>
+      </c>
+      <c r="B33">
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="C33">
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="D33">
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4715400000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>45522</v>
+      </c>
+      <c r="B34">
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="C34">
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="D34">
+        <v>5.4694000000000003</v>
+      </c>
+      <c r="E34">
+        <f>LARGE(B34:D34,1)</f>
+        <v>5.4715400000000001</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>5.4694000000000003</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4708266666666674</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>45523</v>
+      </c>
+      <c r="B35">
+        <v>5.4292999999999996</v>
+      </c>
+      <c r="C35">
+        <v>5.4124999999999996</v>
+      </c>
+      <c r="D35">
+        <v>5.4063999999999997</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>5.4292999999999996</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>5.4063999999999997</v>
+      </c>
+      <c r="G35" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4160666666666657</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>45524</v>
+      </c>
+      <c r="B36">
+        <v>5.4397000000000002</v>
+      </c>
+      <c r="C36">
+        <v>5.4852999999999996</v>
+      </c>
+      <c r="D36">
+        <v>5.4795999999999996</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>5.4852999999999996</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>5.4397000000000002</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4682000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>45525</v>
+      </c>
+      <c r="B37">
+        <v>5.47</v>
+      </c>
+      <c r="C37">
+        <v>5.4812000000000003</v>
+      </c>
+      <c r="D37">
+        <v>5.4836999999999998</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>5.4836999999999998</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>5.47</v>
+      </c>
+      <c r="G37" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4782999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>45526</v>
+      </c>
+      <c r="B38">
+        <v>5.5452000000000004</v>
+      </c>
+      <c r="C38">
+        <v>5.5896999999999997</v>
+      </c>
+      <c r="D38">
+        <v>5.5921000000000003</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>5.5921000000000003</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>5.5452000000000004</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5756666666666668</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>45527</v>
+      </c>
+      <c r="B39">
+        <v>5.5518000000000001</v>
+      </c>
+      <c r="C39">
+        <v>5.4794999999999998</v>
+      </c>
+      <c r="D39">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>5.5518000000000001</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>5.4794999999999998</v>
+      </c>
+      <c r="G39" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5057499999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>45528</v>
+      </c>
+      <c r="B40">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="C40">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="D40">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="G40" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>45529</v>
+      </c>
+      <c r="B41">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="C41">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="D41">
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>5.4859499999999999</v>
+      </c>
+      <c r="G41" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>45530</v>
+      </c>
+      <c r="B42">
+        <v>5.4848999999999997</v>
+      </c>
+      <c r="C42">
+        <v>5.4917999999999996</v>
+      </c>
+      <c r="D42">
+        <v>5.4972000000000003</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>5.4972000000000003</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>5.4848999999999997</v>
+      </c>
+      <c r="G42" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4912999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>45531</v>
+      </c>
+      <c r="B43">
+        <v>5.4927000000000001</v>
+      </c>
+      <c r="C43">
+        <v>5.5025000000000004</v>
+      </c>
+      <c r="D43">
+        <v>5.5094000000000003</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>5.5094000000000003</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>5.4927000000000001</v>
+      </c>
+      <c r="G43" s="6">
+        <f t="shared" si="2"/>
+        <v>5.5015333333333336</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>45532</v>
+      </c>
+      <c r="B44">
+        <v>5.5304000000000002</v>
+      </c>
+      <c r="C44">
+        <v>5.5549799999999996</v>
+      </c>
+      <c r="D44">
+        <v>5.5633999999999997</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>5.5633999999999997</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>5.5304000000000002</v>
+      </c>
+      <c r="G44" s="6">
+        <f t="shared" si="2"/>
+        <v>5.549593333333334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>45533</v>
+      </c>
+      <c r="B45">
+        <v>5.6406000000000001</v>
+      </c>
+      <c r="C45">
+        <v>5.6227</v>
+      </c>
+      <c r="D45">
+        <v>5.6288999999999998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>5.6406000000000001</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>5.6227</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6307333333333345</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>45534</v>
+      </c>
+      <c r="B46">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="C46">
+        <v>5.6341000000000001</v>
+      </c>
+      <c r="D46">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6353600000000013</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>45535</v>
+      </c>
+      <c r="B47">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="C47">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D47">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="G47" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6063799999999988</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>45536</v>
+      </c>
+      <c r="B48">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="C48">
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="D48">
+        <v>5.6116900000000003</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>5.6116900000000003</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>5.6063799999999997</v>
+      </c>
+      <c r="G48" s="6">
+        <f t="shared" si="2"/>
+        <v>5.6081499999999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2 G2" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599224F4-1114-46B0-AF99-277C0227B676}">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>45490</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5.9731800000000002</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5.9967499999999996</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6.0023600000000004</v>
+      </c>
+      <c r="E2">
+        <f>LARGE(B2:D2,1)</f>
+        <v>6.0023600000000004</v>
+      </c>
+      <c r="F2">
+        <f>SMALL(B2:D2,1)</f>
+        <v>5.9731800000000002</v>
+      </c>
+      <c r="G2" s="2">
+        <f>AVERAGE(B2:D2)</f>
+        <v>5.9907633333333337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>45583</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6.00298</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6.0900600000000003</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6.0370799999999996</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E48" si="0">LARGE(B3:D3,1)</f>
+        <v>6.0900600000000003</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F48" si="1">SMALL(B3:D3,1)</f>
+        <v>6.00298</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G48" si="2">AVERAGE(B3:D3)</f>
+        <v>6.0433733333333324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>45584</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6.0396299999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.0720099999999997</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>6.0396299999999998</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="2"/>
+        <v>6.068036666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>45493</v>
+      </c>
+      <c r="B5">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C5">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="D5">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0924699999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>45494</v>
+      </c>
+      <c r="B6">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="C6">
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="D6">
+        <v>6.0363499999999997</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>6.0924699999999996</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>6.0363499999999997</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>6.073763333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>45495</v>
+      </c>
+      <c r="B7">
+        <v>6.0609000000000002</v>
+      </c>
+      <c r="C7">
+        <v>6.06351</v>
+      </c>
+      <c r="D7">
+        <v>6.0671900000000001</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>6.0671900000000001</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>6.0609000000000002</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0638666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>45496</v>
+      </c>
+      <c r="B8">
+        <v>6.0692899999999996</v>
+      </c>
+      <c r="C8">
+        <v>6.0613000000000001</v>
+      </c>
+      <c r="D8">
+        <v>6.0602799999999997</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>6.0692899999999996</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>6.0602799999999997</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0636233333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>45497</v>
+      </c>
+      <c r="B9">
+        <v>6.1232899999999999</v>
+      </c>
+      <c r="C9">
+        <v>6.1300400000000002</v>
+      </c>
+      <c r="D9">
+        <v>6.1289499999999997</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>6.1300400000000002</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>6.1232899999999999</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1274266666666675</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>45498</v>
+      </c>
+      <c r="B10">
+        <v>6.1245200000000004</v>
+      </c>
+      <c r="C10">
+        <v>6.1251600000000002</v>
+      </c>
+      <c r="D10">
+        <v>6.1287700000000003</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>6.1287700000000003</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>6.1245200000000004</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>6.12615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>45499</v>
+      </c>
+      <c r="B11">
+        <v>6.1281999999999996</v>
+      </c>
+      <c r="C11">
+        <v>6.1429999999999998</v>
+      </c>
+      <c r="D11">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>6.1429999999999998</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>6.1281999999999996</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1372233333333339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>45500</v>
+      </c>
+      <c r="B12">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="C12">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="D12">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1404699999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>45501</v>
+      </c>
+      <c r="B13">
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="C13">
+        <v>6.1428500000000001</v>
+      </c>
+      <c r="D13">
+        <v>6.1418600000000003</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>6.1428500000000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>6.1404699999999997</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="2"/>
+        <v>6.141726666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>45502</v>
+      </c>
+      <c r="B14">
+        <v>6.1089200000000003</v>
+      </c>
+      <c r="C14">
+        <v>6.08887</v>
+      </c>
+      <c r="D14">
+        <v>6.0749300000000002</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>6.1089200000000003</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>6.0749300000000002</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0909066666666662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>45503</v>
+      </c>
+      <c r="B15">
+        <v>6.1143400000000003</v>
+      </c>
+      <c r="C15">
+        <v>6.0705400000000003</v>
+      </c>
+      <c r="D15">
+        <v>6.0747400000000003</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>6.1143400000000003</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>6.0705400000000003</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0865399999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>45504</v>
+      </c>
+      <c r="B16">
+        <v>6.15245</v>
+      </c>
+      <c r="C16">
+        <v>6.1144100000000003</v>
+      </c>
+      <c r="D16">
+        <v>6.1261000000000001</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>6.15245</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>6.1144100000000003</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1309866666666677</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>45505</v>
+      </c>
+      <c r="B17">
+        <v>6.0955500000000002</v>
+      </c>
+      <c r="C17">
+        <v>6.1876199999999999</v>
+      </c>
+      <c r="D17">
+        <v>6.2071300000000003</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>6.2071300000000003</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>6.0955500000000002</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1634333333333338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>45506</v>
+      </c>
+      <c r="B18">
+        <v>6.2333999999999996</v>
+      </c>
+      <c r="C18">
+        <v>6.23088</v>
+      </c>
+      <c r="D18">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>6.23088</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="2"/>
+        <v>6.2379500000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>45507</v>
+      </c>
+      <c r="B19">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="C19">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="D19">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="2"/>
+        <v>6.2495700000000012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>45508</v>
+      </c>
+      <c r="B20">
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="C20">
+        <v>6.2564099999999998</v>
+      </c>
+      <c r="D20">
+        <v>6.25481</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>6.2564099999999998</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>6.2495700000000003</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="2"/>
+        <v>6.2535966666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>45509</v>
+      </c>
+      <c r="B21">
+        <v>6.3701999999999996</v>
+      </c>
+      <c r="C21">
+        <v>6.2915599999999996</v>
+      </c>
+      <c r="D21">
+        <v>6.2695499999999997</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>6.3701999999999996</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>6.2695499999999997</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="2"/>
+        <v>6.3104366666666669</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>45510</v>
+      </c>
+      <c r="B22">
+        <v>6.1828000000000003</v>
+      </c>
+      <c r="C22">
+        <v>6.1848700000000001</v>
+      </c>
+      <c r="D22">
+        <v>6.1767700000000003</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>6.1848700000000001</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>6.1767700000000003</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1814800000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>45511</v>
+      </c>
+      <c r="B23">
+        <v>6.1179699999999997</v>
+      </c>
+      <c r="C23">
+        <v>6.1429999999999998</v>
+      </c>
+      <c r="D23">
+        <v>6.1602499999999996</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>6.1602499999999996</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>6.1179699999999997</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1404066666666663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>45512</v>
+      </c>
+      <c r="B24">
+        <v>6.1177400000000004</v>
+      </c>
+      <c r="C24">
+        <v>6.0851300000000004</v>
+      </c>
+      <c r="D24">
+        <v>6.0570500000000003</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>6.1177400000000004</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>6.0570500000000003</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0866400000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>45513</v>
+      </c>
+      <c r="B25">
+        <v>6.0171000000000001</v>
+      </c>
+      <c r="C25">
+        <v>6.0211600000000001</v>
+      </c>
+      <c r="D25">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>6.0211600000000001</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0172700000000008</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>45514</v>
+      </c>
+      <c r="B26">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="C26">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="D26">
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>6.0135500000000004</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0135499999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>45515</v>
+      </c>
+      <c r="B27">
+        <v>6.0078100000000001</v>
+      </c>
+      <c r="C27">
+        <v>6.0093300000000003</v>
+      </c>
+      <c r="D27">
+        <v>6.0075200000000004</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>6.0093300000000003</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>6.0075200000000004</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0082200000000006</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>45516</v>
+      </c>
+      <c r="B28">
+        <v>6.0078100000000001</v>
+      </c>
+      <c r="C28">
+        <v>6.0093300000000003</v>
+      </c>
+      <c r="D28">
+        <v>6.0075200000000004</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>6.0093300000000003</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>6.0075200000000004</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0082200000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>45517</v>
+      </c>
+      <c r="B29">
+        <v>6.0146800000000002</v>
+      </c>
+      <c r="C29">
+        <v>5.9917600000000002</v>
+      </c>
+      <c r="D29">
+        <v>5.9986600000000001</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>6.0146800000000002</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>5.9917600000000002</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0017000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>45518</v>
+      </c>
+      <c r="B30">
+        <v>6.0144599999999997</v>
+      </c>
+      <c r="C30">
+        <v>6.0229699999999999</v>
+      </c>
+      <c r="D30">
+        <v>6.0214800000000004</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>6.0229699999999999</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>6.0144599999999997</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>6.019636666666667</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>45519</v>
+      </c>
+      <c r="B31">
+        <v>5.9838699999999996</v>
+      </c>
+      <c r="C31">
+        <v>6.0173199999999998</v>
+      </c>
+      <c r="D31">
+        <v>6.0248200000000001</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>6.0248200000000001</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>5.9838699999999996</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0086699999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>45520</v>
+      </c>
+      <c r="B32">
+        <v>6.0010300000000001</v>
+      </c>
+      <c r="C32">
+        <v>6.0262700000000002</v>
+      </c>
+      <c r="D32">
+        <v>6.03376</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>6.03376</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>6.0010300000000001</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0203533333333334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>45521</v>
+      </c>
+      <c r="B33">
+        <v>6.03376</v>
+      </c>
+      <c r="C33">
+        <v>6.03376</v>
+      </c>
+      <c r="D33">
+        <v>6.03376</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>6.03376</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>6.03376</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="2"/>
+        <v>6.03376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>45522</v>
+      </c>
+      <c r="B34">
+        <v>6.03376</v>
+      </c>
+      <c r="C34">
+        <v>6.03376</v>
+      </c>
+      <c r="D34">
+        <v>6.0332999999999997</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>6.03376</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>6.0332999999999997</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0336066666666666</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>45523</v>
+      </c>
+      <c r="B35">
+        <v>5.9958999999999998</v>
+      </c>
+      <c r="C35">
+        <v>5.9989999999999997</v>
+      </c>
+      <c r="D35">
+        <v>5.9932999999999996</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>5.9989999999999997</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>5.9932999999999996</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="2"/>
+        <v>5.9960666666666667</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>45524</v>
+      </c>
+      <c r="B36">
+        <v>6.0391000000000004</v>
+      </c>
+      <c r="C36">
+        <v>6.1021000000000001</v>
+      </c>
+      <c r="D36">
+        <v>6.0941000000000001</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>6.1021000000000001</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>6.0391000000000004</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0784333333333338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>45525</v>
+      </c>
+      <c r="B37">
+        <v>6.0796000000000001</v>
+      </c>
+      <c r="C37">
+        <v>6.1125999999999996</v>
+      </c>
+      <c r="D37">
+        <v>6.1108000000000002</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>6.1125999999999996</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>6.0796000000000001</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="2"/>
+        <v>6.101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>45526</v>
+      </c>
+      <c r="B38">
+        <v>6.1086999999999998</v>
+      </c>
+      <c r="C38">
+        <v>6.2092999999999998</v>
+      </c>
+      <c r="D38">
+        <v>6.2225999999999999</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>6.2225999999999999</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>6.1086999999999998</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1801999999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>45527</v>
+      </c>
+      <c r="B39">
+        <v>6.1725000000000003</v>
+      </c>
+      <c r="C39">
+        <v>6.1323999999999996</v>
+      </c>
+      <c r="D39">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>6.1725000000000003</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>6.1323999999999996</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1483566666666674</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>45528</v>
+      </c>
+      <c r="B40">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="C40">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="D40">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1401700000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>45529</v>
+      </c>
+      <c r="B41">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="C41">
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="D41">
+        <v>6.1395999999999997</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>6.1401700000000003</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>6.1395999999999997</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1399800000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>45530</v>
+      </c>
+      <c r="B42">
+        <v>6.1208999999999998</v>
+      </c>
+      <c r="C42">
+        <v>6.1284999999999998</v>
+      </c>
+      <c r="D42">
+        <v>6.1401000000000003</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>6.1401000000000003</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>6.1208999999999998</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="2"/>
+        <v>6.129833333333333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>45531</v>
+      </c>
+      <c r="B43">
+        <v>6.1345000000000001</v>
+      </c>
+      <c r="C43">
+        <v>6.1538000000000004</v>
+      </c>
+      <c r="D43">
+        <v>6.1562000000000001</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>6.1562000000000001</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>6.1345000000000001</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1481666666666657</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>45532</v>
+      </c>
+      <c r="B44">
+        <v>6.1444999999999999</v>
+      </c>
+      <c r="C44">
+        <v>6.1733000000000002</v>
+      </c>
+      <c r="D44">
+        <v>6.1912000000000003</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>6.1912000000000003</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>6.1444999999999999</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1696666666666671</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>45533</v>
+      </c>
+      <c r="B45">
+        <v>6.2511999999999999</v>
+      </c>
+      <c r="C45">
+        <v>6.2274000000000003</v>
+      </c>
+      <c r="D45">
+        <v>6.2314999999999996</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>6.2511999999999999</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>6.2274000000000003</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="2"/>
+        <v>6.2366999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>45534</v>
+      </c>
+      <c r="B46">
+        <v>6.2614000000000001</v>
+      </c>
+      <c r="C46">
+        <v>6.2282000000000002</v>
+      </c>
+      <c r="D46">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>6.2614000000000001</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="2"/>
+        <v>6.2276566666666655</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>45535</v>
+      </c>
+      <c r="B47">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C47">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="D47">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1933699999999989</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>45536</v>
+      </c>
+      <c r="B48">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="C48">
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="D48">
+        <v>6.2034399999999996</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>6.2034399999999996</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>6.1933699999999998</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="2"/>
+        <v>6.1967266666666667</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
adds typings to the columns
</commit_message>
<xml_diff>
--- a/excel/exchanges_historic_series.xlsx
+++ b/excel/exchanges_historic_series.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D8B1E1-06AD-49B7-A03A-544A83B7F47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4796C26-B19C-4701-BCBE-DF4127F1899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -153,6 +153,9 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4051,66 +4054,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47E47A6-69F4-4AEB-9879-64F1134C7037}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="9" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="11.5703125" style="6" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>45490</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>5.4586899999999998</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>5.4864600000000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>5.4898899999999999</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <f>LARGE(C2:E2,1)</f>
         <v>5.4898899999999999</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <f>SMALL(C2:E2,1)</f>
         <v>5.4586899999999998</v>
       </c>
@@ -4120,26 +4125,26 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>45583</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>5.4920900000000001</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>5.5887500000000001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>5.5447100000000002</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <f t="shared" ref="F3:F48" si="0">LARGE(C3:E3,1)</f>
         <v>5.5887500000000001</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <f t="shared" ref="G3:G48" si="1">SMALL(C3:E3,1)</f>
         <v>5.4920900000000001</v>
       </c>
@@ -4149,26 +4154,26 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>45584</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>5.5445000000000002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>5.5788599999999997</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>5.59816</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <f t="shared" si="0"/>
         <v>5.59816</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <f t="shared" si="1"/>
         <v>5.5445000000000002</v>
       </c>
@@ -4178,26 +4183,26 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>45493</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>5.59816</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>5.59816</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>5.59816</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <f t="shared" si="0"/>
         <v>5.59816</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>5.59816</v>
       </c>
@@ -4207,26 +4212,26 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>45494</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>5.59816</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>5.59816</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>5.5453000000000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>5.59816</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <f t="shared" si="1"/>
         <v>5.5453000000000001</v>
       </c>
@@ -4236,26 +4241,26 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>45495</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>5.5717100000000004</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>5.5692599999999999</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>5.5720900000000002</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>5.5720900000000002</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>5.5692599999999999</v>
       </c>
@@ -4265,26 +4270,26 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>45496</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>5.5933099999999998</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>5.5861900000000002</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>5.5865600000000004</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>5.5933099999999998</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>5.5861900000000002</v>
       </c>
@@ -4294,26 +4299,26 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>45497</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>5.6412399999999998</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>5.6542899999999996</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>5.6550500000000001</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>5.6550500000000001</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>5.6412399999999998</v>
       </c>
@@ -4323,26 +4328,26 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>45498</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>5.6501999999999999</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>5.64764</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>5.6452499999999999</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
         <v>5.6501999999999999</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>5.6452499999999999</v>
       </c>
@@ -4352,26 +4357,26 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>45499</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>5.6402900000000002</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>5.6578400000000002</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>5.6562999999999999</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>5.6578400000000002</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>5.6402900000000002</v>
       </c>
@@ -4381,26 +4386,26 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>45500</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>5.6562999999999999</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>5.6562999999999999</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>5.6562999999999999</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <f t="shared" si="0"/>
         <v>5.6562999999999999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>5.6562999999999999</v>
       </c>
@@ -4410,26 +4415,26 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>45501</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>5.6562999999999999</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="6">
         <v>5.65665</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>5.6568100000000001</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <f t="shared" si="0"/>
         <v>5.6568100000000001</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="6">
         <f t="shared" si="1"/>
         <v>5.6562999999999999</v>
       </c>
@@ -4439,26 +4444,26 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>45502</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>5.6509</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>5.6242999999999999</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>5.6160800000000002</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
         <v>5.6509</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <f t="shared" si="1"/>
         <v>5.6160800000000002</v>
       </c>
@@ -4468,26 +4473,26 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" s="5">
         <v>45503</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>5.6556600000000001</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>5.6123000000000003</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>5.6125499999999997</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="6">
         <f t="shared" si="0"/>
         <v>5.6556600000000001</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="6">
         <f t="shared" si="1"/>
         <v>5.6123000000000003</v>
       </c>
@@ -4497,26 +4502,26 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
       <c r="B16" s="5">
         <v>45504</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>5.6746600000000003</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>5.6479900000000001</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="6">
         <v>5.6578999999999997</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="6">
         <f t="shared" si="0"/>
         <v>5.6746600000000003</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="6">
         <f t="shared" si="1"/>
         <v>5.6479900000000001</v>
       </c>
@@ -4526,26 +4531,26 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>45505</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>5.6421900000000003</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>5.7348699999999999</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>5.7524199999999999</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="6">
         <f t="shared" si="0"/>
         <v>5.7524199999999999</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="6">
         <f t="shared" si="1"/>
         <v>5.6421900000000003</v>
       </c>
@@ -4555,26 +4560,26 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="5">
         <v>45506</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>5.7158499999999997</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>5.7095900000000004</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>5.7280699999999998</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="6">
         <f t="shared" si="0"/>
         <v>5.7280699999999998</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <f t="shared" si="1"/>
         <v>5.7095900000000004</v>
       </c>
@@ -4584,26 +4589,26 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>45507</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>5.7280699999999998</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>5.7280699999999998</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="6">
         <v>5.7280699999999998</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="6">
         <f t="shared" si="0"/>
         <v>5.7280699999999998</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="6">
         <f t="shared" si="1"/>
         <v>5.7280699999999998</v>
       </c>
@@ -4613,26 +4618,26 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
       <c r="B20" s="5">
         <v>45508</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>5.7280699999999998</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>5.7272100000000004</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <v>5.7281000000000004</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="6">
         <f t="shared" si="0"/>
         <v>5.7281000000000004</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="6">
         <f t="shared" si="1"/>
         <v>5.7272100000000004</v>
       </c>
@@ -4642,26 +4647,26 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>45509</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>5.8010999999999999</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>5.7407599999999999</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>5.7229799999999997</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="6">
         <f t="shared" si="0"/>
         <v>5.8010999999999999</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="6">
         <f t="shared" si="1"/>
         <v>5.7229799999999997</v>
       </c>
@@ -4671,26 +4676,26 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>45510</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>5.6627099999999997</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>5.6586100000000004</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <v>5.6571600000000002</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <f t="shared" si="0"/>
         <v>5.6627099999999997</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="6">
         <f t="shared" si="1"/>
         <v>5.6571600000000002</v>
       </c>
@@ -4700,26 +4705,26 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
       <c r="B23" s="5">
         <v>45511</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>5.6033099999999996</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>5.6236600000000001</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>5.6373899999999999</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <f t="shared" si="0"/>
         <v>5.6373899999999999</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="6">
         <f t="shared" si="1"/>
         <v>5.6033099999999996</v>
       </c>
@@ -4729,26 +4734,26 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
       <c r="B24" s="5">
         <v>45512</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>5.617</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>5.5742599999999998</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="6">
         <v>5.5475099999999999</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <f t="shared" si="0"/>
         <v>5.617</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="6">
         <f t="shared" si="1"/>
         <v>5.5475099999999999</v>
       </c>
@@ -4758,26 +4763,26 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
       <c r="B25" s="5">
         <v>45513</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>5.5172400000000001</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>5.5146600000000001</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="6">
         <v>5.5087000000000002</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <f t="shared" si="0"/>
         <v>5.5172400000000001</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="6">
         <f t="shared" si="1"/>
         <v>5.5087000000000002</v>
       </c>
@@ -4787,26 +4792,26 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
       <c r="B26" s="5">
         <v>45514</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>5.5087000000000002</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>5.5087000000000002</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="6">
         <v>5.5087000000000002</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="6">
         <f t="shared" si="0"/>
         <v>5.5087000000000002</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="6">
         <f t="shared" si="1"/>
         <v>5.5087000000000002</v>
       </c>
@@ -4816,26 +4821,26 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="5">
         <v>45515</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>5.4993999999999996</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>5.4977400000000003</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="6">
         <v>5.4938399999999996</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="6">
         <f t="shared" si="0"/>
         <v>5.4993999999999996</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="6">
         <f t="shared" si="1"/>
         <v>5.4938399999999996</v>
       </c>
@@ -4845,26 +4850,26 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
       <c r="B28" s="5">
         <v>45516</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>5.4993999999999996</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>5.4877399999999996</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="6">
         <v>5.4938399999999996</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="6">
         <f t="shared" si="0"/>
         <v>5.4993999999999996</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="6">
         <f t="shared" si="1"/>
         <v>5.4877399999999996</v>
       </c>
@@ -4874,26 +4879,26 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
       <c r="B29" s="5">
         <v>45517</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>5.4891100000000002</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>5.4487899999999998</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <v>5.4572900000000004</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="6">
         <f t="shared" si="0"/>
         <v>5.4891100000000002</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
         <f t="shared" si="1"/>
         <v>5.4487899999999998</v>
       </c>
@@ -4903,26 +4908,26 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
       <c r="B30" s="5">
         <v>45518</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>5.44909</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>5.46896</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="6">
         <v>5.4706099999999998</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="6">
         <f t="shared" si="0"/>
         <v>5.4706099999999998</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="6">
         <f t="shared" si="1"/>
         <v>5.44909</v>
       </c>
@@ -4932,26 +4937,26 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
       <c r="B31" s="5">
         <v>45519</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>5.4555100000000003</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>5.4836900000000002</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="6">
         <v>5.4863400000000002</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="6">
         <f t="shared" si="0"/>
         <v>5.4863400000000002</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="6">
         <f t="shared" si="1"/>
         <v>5.4555100000000003</v>
       </c>
@@ -4961,26 +4966,26 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
       <c r="B32" s="5">
         <v>45520</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>5.4542599999999997</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>5.46624</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="6">
         <v>5.4715400000000001</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="6">
         <f t="shared" si="0"/>
         <v>5.4715400000000001</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="6">
         <f t="shared" si="1"/>
         <v>5.4542599999999997</v>
       </c>
@@ -4990,26 +4995,26 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
       <c r="B33" s="5">
         <v>45521</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="6">
         <v>5.4715400000000001</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="6">
         <v>5.4715400000000001</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="6">
         <v>5.4715400000000001</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="6">
         <f t="shared" si="0"/>
         <v>5.4715400000000001</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="6">
         <f t="shared" si="1"/>
         <v>5.4715400000000001</v>
       </c>
@@ -5019,26 +5024,26 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
       <c r="B34" s="5">
         <v>45522</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <v>5.4715400000000001</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="6">
         <v>5.4715400000000001</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="6">
         <v>5.4694000000000003</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="6">
         <f>LARGE(C34:E34,1)</f>
         <v>5.4715400000000001</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="6">
         <f t="shared" si="1"/>
         <v>5.4694000000000003</v>
       </c>
@@ -5048,26 +5053,26 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
       <c r="B35" s="5">
         <v>45523</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>5.4292999999999996</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="6">
         <v>5.4124999999999996</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="6">
         <v>5.4063999999999997</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="6">
         <f t="shared" si="0"/>
         <v>5.4292999999999996</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="6">
         <f t="shared" si="1"/>
         <v>5.4063999999999997</v>
       </c>
@@ -5077,26 +5082,26 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
       <c r="B36" s="5">
         <v>45524</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <v>5.4397000000000002</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>5.4852999999999996</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="6">
         <v>5.4795999999999996</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="6">
         <f t="shared" si="0"/>
         <v>5.4852999999999996</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="6">
         <f t="shared" si="1"/>
         <v>5.4397000000000002</v>
       </c>
@@ -5106,26 +5111,26 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="9">
         <v>36</v>
       </c>
       <c r="B37" s="5">
         <v>45525</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>5.47</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="6">
         <v>5.4812000000000003</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="6">
         <v>5.4836999999999998</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="6">
         <f t="shared" si="0"/>
         <v>5.4836999999999998</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="6">
         <f t="shared" si="1"/>
         <v>5.47</v>
       </c>
@@ -5135,26 +5140,26 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="9">
         <v>37</v>
       </c>
       <c r="B38" s="5">
         <v>45526</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="6">
         <v>5.5452000000000004</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="6">
         <v>5.5896999999999997</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="6">
         <v>5.5921000000000003</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="6">
         <f t="shared" si="0"/>
         <v>5.5921000000000003</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="6">
         <f t="shared" si="1"/>
         <v>5.5452000000000004</v>
       </c>
@@ -5164,26 +5169,26 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="9">
         <v>38</v>
       </c>
       <c r="B39" s="5">
         <v>45527</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="6">
         <v>5.5518000000000001</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="6">
         <v>5.4794999999999998</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="6">
         <v>5.4859499999999999</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="6">
         <f t="shared" si="0"/>
         <v>5.5518000000000001</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="6">
         <f t="shared" si="1"/>
         <v>5.4794999999999998</v>
       </c>
@@ -5193,26 +5198,26 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="9">
         <v>39</v>
       </c>
       <c r="B40" s="5">
         <v>45528</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <v>5.4859499999999999</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>5.4859499999999999</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="6">
         <v>5.4859499999999999</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="6">
         <f t="shared" si="0"/>
         <v>5.4859499999999999</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="6">
         <f t="shared" si="1"/>
         <v>5.4859499999999999</v>
       </c>
@@ -5222,26 +5227,26 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="9">
         <v>40</v>
       </c>
       <c r="B41" s="5">
         <v>45529</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>5.4859499999999999</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>5.4859499999999999</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="6">
         <v>5.4859499999999999</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="6">
         <f t="shared" si="0"/>
         <v>5.4859499999999999</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="6">
         <f t="shared" si="1"/>
         <v>5.4859499999999999</v>
       </c>
@@ -5251,26 +5256,26 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="9">
         <v>41</v>
       </c>
       <c r="B42" s="5">
         <v>45530</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="6">
         <v>5.4848999999999997</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="6">
         <v>5.4917999999999996</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="6">
         <v>5.4972000000000003</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="6">
         <f t="shared" si="0"/>
         <v>5.4972000000000003</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="6">
         <f t="shared" si="1"/>
         <v>5.4848999999999997</v>
       </c>
@@ -5280,26 +5285,26 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="9">
         <v>42</v>
       </c>
       <c r="B43" s="5">
         <v>45531</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="6">
         <v>5.4927000000000001</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="6">
         <v>5.5025000000000004</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="6">
         <v>5.5094000000000003</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="6">
         <f t="shared" si="0"/>
         <v>5.5094000000000003</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="6">
         <f t="shared" si="1"/>
         <v>5.4927000000000001</v>
       </c>
@@ -5309,26 +5314,26 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="9">
         <v>43</v>
       </c>
       <c r="B44" s="5">
         <v>45532</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="6">
         <v>5.5304000000000002</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="6">
         <v>5.5549799999999996</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="6">
         <v>5.5633999999999997</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="6">
         <f t="shared" si="0"/>
         <v>5.5633999999999997</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="6">
         <f t="shared" si="1"/>
         <v>5.5304000000000002</v>
       </c>
@@ -5338,26 +5343,26 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="9">
         <v>44</v>
       </c>
       <c r="B45" s="5">
         <v>45533</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="6">
         <v>5.6406000000000001</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="6">
         <v>5.6227</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="6">
         <v>5.6288999999999998</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="6">
         <f t="shared" si="0"/>
         <v>5.6406000000000001</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="6">
         <f t="shared" si="1"/>
         <v>5.6227</v>
       </c>
@@ -5367,26 +5372,26 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="9">
         <v>45</v>
       </c>
       <c r="B46" s="5">
         <v>45534</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="6">
         <v>5.6656000000000004</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="6">
         <v>5.6341000000000001</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="6">
         <v>5.6063799999999997</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="6">
         <f t="shared" si="0"/>
         <v>5.6656000000000004</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="6">
         <f t="shared" si="1"/>
         <v>5.6063799999999997</v>
       </c>
@@ -5396,26 +5401,26 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="9">
         <v>46</v>
       </c>
       <c r="B47" s="5">
         <v>45535</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="6">
         <v>5.6063799999999997</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="6">
         <v>5.6063799999999997</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="6">
         <v>5.6063799999999997</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="6">
         <f t="shared" si="0"/>
         <v>5.6063799999999997</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="6">
         <f t="shared" si="1"/>
         <v>5.6063799999999997</v>
       </c>
@@ -5425,26 +5430,26 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="9">
         <v>47</v>
       </c>
       <c r="B48" s="5">
         <v>45536</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="6">
         <v>5.6063799999999997</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="6">
         <v>5.6063799999999997</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="6">
         <v>5.6116900000000003</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="6">
         <f t="shared" si="0"/>
         <v>5.6116900000000003</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="6">
         <f t="shared" si="1"/>
         <v>5.6063799999999997</v>
       </c>
@@ -5452,12 +5457,6 @@
         <f t="shared" si="2"/>
         <v>5.6081499999999993</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5472,1401 +5471,1403 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="9" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="11.7109375" style="6" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>45490</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="6">
         <v>5.9731800000000002</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>5.9967499999999996</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="6">
         <v>6.0023600000000004</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <f>LARGE(C2:E2,1)</f>
         <v>6.0023600000000004</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <f>SMALL(C2:E2,1)</f>
         <v>5.9731800000000002</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="6">
         <f>AVERAGE(C2:E2)</f>
         <v>5.9907633333333337</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>45583</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="6">
         <v>6.00298</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>6.0900600000000003</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="6">
         <v>6.0370799999999996</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <f t="shared" ref="F3:F48" si="0">LARGE(C3:E3,1)</f>
         <v>6.0900600000000003</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <f t="shared" ref="G3:G48" si="1">SMALL(C3:E3,1)</f>
         <v>6.00298</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="6">
         <f t="shared" ref="H3:H48" si="2">AVERAGE(C3:E3)</f>
         <v>6.0433733333333324</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>45584</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="6">
         <v>6.0396299999999998</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="6">
         <v>6.0720099999999997</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="6">
         <v>6.0924699999999996</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <f t="shared" si="0"/>
         <v>6.0924699999999996</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <f t="shared" si="1"/>
         <v>6.0396299999999998</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="6">
         <f t="shared" si="2"/>
         <v>6.068036666666667</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>45493</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>6.0924699999999996</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>6.0924699999999996</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>6.0924699999999996</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <f t="shared" si="0"/>
         <v>6.0924699999999996</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>6.0924699999999996</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="6">
         <f t="shared" si="2"/>
         <v>6.0924699999999996</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>45494</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>6.0924699999999996</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>6.0924699999999996</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>6.0363499999999997</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>6.0924699999999996</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <f t="shared" si="1"/>
         <v>6.0363499999999997</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="6">
         <f t="shared" si="2"/>
         <v>6.073763333333333</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>45495</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>6.0609000000000002</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>6.06351</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>6.0671900000000001</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>6.0671900000000001</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>6.0609000000000002</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="6">
         <f t="shared" si="2"/>
         <v>6.0638666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>45496</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>6.0692899999999996</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>6.0613000000000001</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>6.0602799999999997</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>6.0692899999999996</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>6.0602799999999997</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="6">
         <f t="shared" si="2"/>
         <v>6.0636233333333331</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>45497</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>6.1232899999999999</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>6.1300400000000002</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>6.1289499999999997</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>6.1300400000000002</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>6.1232899999999999</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="6">
         <f t="shared" si="2"/>
         <v>6.1274266666666675</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>45498</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>6.1245200000000004</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>6.1251600000000002</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>6.1287700000000003</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
         <v>6.1287700000000003</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>6.1245200000000004</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="6">
         <f t="shared" si="2"/>
         <v>6.12615</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>45499</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>6.1281999999999996</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>6.1429999999999998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>6.1404699999999997</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>6.1429999999999998</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>6.1281999999999996</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="6">
         <f t="shared" si="2"/>
         <v>6.1372233333333339</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>45500</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>6.1404699999999997</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>6.1404699999999997</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>6.1404699999999997</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <f t="shared" si="0"/>
         <v>6.1404699999999997</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>6.1404699999999997</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="6">
         <f t="shared" si="2"/>
         <v>6.1404699999999997</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>45501</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>6.1404699999999997</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="6">
         <v>6.1428500000000001</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>6.1418600000000003</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <f t="shared" si="0"/>
         <v>6.1428500000000001</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="6">
         <f t="shared" si="1"/>
         <v>6.1404699999999997</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="6">
         <f t="shared" si="2"/>
         <v>6.141726666666667</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>45502</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>6.1089200000000003</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>6.08887</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>6.0749300000000002</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
         <v>6.1089200000000003</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <f t="shared" si="1"/>
         <v>6.0749300000000002</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="6">
         <f t="shared" si="2"/>
         <v>6.0909066666666662</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" s="5">
         <v>45503</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>6.1143400000000003</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>6.0705400000000003</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>6.0747400000000003</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="6">
         <f t="shared" si="0"/>
         <v>6.1143400000000003</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="6">
         <f t="shared" si="1"/>
         <v>6.0705400000000003</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="6">
         <f t="shared" si="2"/>
         <v>6.0865399999999994</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
       <c r="B16" s="5">
         <v>45504</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>6.15245</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>6.1144100000000003</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="6">
         <v>6.1261000000000001</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="6">
         <f t="shared" si="0"/>
         <v>6.15245</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="6">
         <f t="shared" si="1"/>
         <v>6.1144100000000003</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="6">
         <f t="shared" si="2"/>
         <v>6.1309866666666677</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>45505</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>6.0955500000000002</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>6.1876199999999999</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>6.2071300000000003</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="6">
         <f t="shared" si="0"/>
         <v>6.2071300000000003</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="6">
         <f t="shared" si="1"/>
         <v>6.0955500000000002</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="6">
         <f t="shared" si="2"/>
         <v>6.1634333333333338</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="5">
         <v>45506</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>6.2333999999999996</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>6.23088</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>6.2495700000000003</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="6">
         <f t="shared" si="0"/>
         <v>6.2495700000000003</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <f t="shared" si="1"/>
         <v>6.23088</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="6">
         <f t="shared" si="2"/>
         <v>6.2379500000000005</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>45507</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>6.2495700000000003</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>6.2495700000000003</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="6">
         <v>6.2495700000000003</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="6">
         <f t="shared" si="0"/>
         <v>6.2495700000000003</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="6">
         <f t="shared" si="1"/>
         <v>6.2495700000000003</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="6">
         <f t="shared" si="2"/>
         <v>6.2495700000000012</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
       <c r="B20" s="5">
         <v>45508</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>6.2495700000000003</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>6.2564099999999998</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <v>6.25481</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="6">
         <f t="shared" si="0"/>
         <v>6.2564099999999998</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="6">
         <f t="shared" si="1"/>
         <v>6.2495700000000003</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="6">
         <f t="shared" si="2"/>
         <v>6.2535966666666667</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>45509</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>6.3701999999999996</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>6.2915599999999996</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>6.2695499999999997</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="6">
         <f t="shared" si="0"/>
         <v>6.3701999999999996</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="6">
         <f t="shared" si="1"/>
         <v>6.2695499999999997</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="6">
         <f t="shared" si="2"/>
         <v>6.3104366666666669</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>45510</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>6.1828000000000003</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>6.1848700000000001</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <v>6.1767700000000003</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <f t="shared" si="0"/>
         <v>6.1848700000000001</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="6">
         <f t="shared" si="1"/>
         <v>6.1767700000000003</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="6">
         <f t="shared" si="2"/>
         <v>6.1814800000000005</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
       <c r="B23" s="5">
         <v>45511</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>6.1179699999999997</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>6.1429999999999998</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>6.1602499999999996</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <f t="shared" si="0"/>
         <v>6.1602499999999996</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="6">
         <f t="shared" si="1"/>
         <v>6.1179699999999997</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="6">
         <f t="shared" si="2"/>
         <v>6.1404066666666663</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
       <c r="B24" s="5">
         <v>45512</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>6.1177400000000004</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>6.0851300000000004</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="6">
         <v>6.0570500000000003</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <f t="shared" si="0"/>
         <v>6.1177400000000004</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="6">
         <f t="shared" si="1"/>
         <v>6.0570500000000003</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="6">
         <f t="shared" si="2"/>
         <v>6.0866400000000001</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
       <c r="B25" s="5">
         <v>45513</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>6.0171000000000001</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>6.0211600000000001</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="6">
         <v>6.0135500000000004</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <f t="shared" si="0"/>
         <v>6.0211600000000001</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="6">
         <f t="shared" si="1"/>
         <v>6.0135500000000004</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="6">
         <f t="shared" si="2"/>
         <v>6.0172700000000008</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
       <c r="B26" s="5">
         <v>45514</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>6.0135500000000004</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>6.0135500000000004</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="6">
         <v>6.0135500000000004</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="6">
         <f t="shared" si="0"/>
         <v>6.0135500000000004</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="6">
         <f t="shared" si="1"/>
         <v>6.0135500000000004</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="6">
         <f t="shared" si="2"/>
         <v>6.0135499999999995</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="5">
         <v>45515</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>6.0078100000000001</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>6.0093300000000003</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="6">
         <v>6.0075200000000004</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="6">
         <f t="shared" si="0"/>
         <v>6.0093300000000003</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="6">
         <f t="shared" si="1"/>
         <v>6.0075200000000004</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="6">
         <f t="shared" si="2"/>
         <v>6.0082200000000006</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
       <c r="B28" s="5">
         <v>45516</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>6.0078100000000001</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>6.0093300000000003</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="6">
         <v>6.0075200000000004</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="6">
         <f t="shared" si="0"/>
         <v>6.0093300000000003</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="6">
         <f t="shared" si="1"/>
         <v>6.0075200000000004</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="6">
         <f t="shared" si="2"/>
         <v>6.0082200000000006</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
       <c r="B29" s="5">
         <v>45517</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>6.0146800000000002</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>5.9917600000000002</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <v>5.9986600000000001</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="6">
         <f t="shared" si="0"/>
         <v>6.0146800000000002</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
         <f t="shared" si="1"/>
         <v>5.9917600000000002</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="6">
         <f t="shared" si="2"/>
         <v>6.0017000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
       <c r="B30" s="5">
         <v>45518</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>6.0144599999999997</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>6.0229699999999999</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="6">
         <v>6.0214800000000004</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="6">
         <f t="shared" si="0"/>
         <v>6.0229699999999999</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="6">
         <f t="shared" si="1"/>
         <v>6.0144599999999997</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="6">
         <f t="shared" si="2"/>
         <v>6.019636666666667</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
       <c r="B31" s="5">
         <v>45519</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>5.9838699999999996</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>6.0173199999999998</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="6">
         <v>6.0248200000000001</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="6">
         <f t="shared" si="0"/>
         <v>6.0248200000000001</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="6">
         <f t="shared" si="1"/>
         <v>5.9838699999999996</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="6">
         <f t="shared" si="2"/>
         <v>6.0086699999999995</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
       <c r="B32" s="5">
         <v>45520</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>6.0010300000000001</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>6.0262700000000002</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="6">
         <v>6.03376</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="6">
         <f t="shared" si="0"/>
         <v>6.03376</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="6">
         <f t="shared" si="1"/>
         <v>6.0010300000000001</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="6">
         <f t="shared" si="2"/>
         <v>6.0203533333333334</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
       <c r="B33" s="5">
         <v>45521</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="6">
         <v>6.03376</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="6">
         <v>6.03376</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="6">
         <v>6.03376</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="6">
         <f t="shared" si="0"/>
         <v>6.03376</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="6">
         <f t="shared" si="1"/>
         <v>6.03376</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="6">
         <f t="shared" si="2"/>
         <v>6.03376</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
       <c r="B34" s="5">
         <v>45522</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <v>6.03376</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="6">
         <v>6.03376</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="6">
         <v>6.0332999999999997</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="6">
         <f t="shared" si="0"/>
         <v>6.03376</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="6">
         <f t="shared" si="1"/>
         <v>6.0332999999999997</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="6">
         <f t="shared" si="2"/>
         <v>6.0336066666666666</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
       <c r="B35" s="5">
         <v>45523</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>5.9958999999999998</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="6">
         <v>5.9989999999999997</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="6">
         <v>5.9932999999999996</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="6">
         <f t="shared" si="0"/>
         <v>5.9989999999999997</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="6">
         <f t="shared" si="1"/>
         <v>5.9932999999999996</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="6">
         <f t="shared" si="2"/>
         <v>5.9960666666666667</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
       <c r="B36" s="5">
         <v>45524</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <v>6.0391000000000004</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>6.1021000000000001</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="6">
         <v>6.0941000000000001</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="6">
         <f t="shared" si="0"/>
         <v>6.1021000000000001</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="6">
         <f t="shared" si="1"/>
         <v>6.0391000000000004</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="6">
         <f t="shared" si="2"/>
         <v>6.0784333333333338</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="9">
         <v>36</v>
       </c>
       <c r="B37" s="5">
         <v>45525</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>6.0796000000000001</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="6">
         <v>6.1125999999999996</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="6">
         <v>6.1108000000000002</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="6">
         <f t="shared" si="0"/>
         <v>6.1125999999999996</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="6">
         <f t="shared" si="1"/>
         <v>6.0796000000000001</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="6">
         <f t="shared" si="2"/>
         <v>6.101</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="9">
         <v>37</v>
       </c>
       <c r="B38" s="5">
         <v>45526</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="6">
         <v>6.1086999999999998</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="6">
         <v>6.2092999999999998</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="6">
         <v>6.2225999999999999</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="6">
         <f t="shared" si="0"/>
         <v>6.2225999999999999</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="6">
         <f t="shared" si="1"/>
         <v>6.1086999999999998</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="6">
         <f t="shared" si="2"/>
         <v>6.1801999999999992</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="9">
         <v>38</v>
       </c>
       <c r="B39" s="5">
         <v>45527</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="6">
         <v>6.1725000000000003</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="6">
         <v>6.1323999999999996</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="6">
         <v>6.1401700000000003</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="6">
         <f t="shared" si="0"/>
         <v>6.1725000000000003</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="6">
         <f t="shared" si="1"/>
         <v>6.1323999999999996</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="6">
         <f t="shared" si="2"/>
         <v>6.1483566666666674</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="9">
         <v>39</v>
       </c>
       <c r="B40" s="5">
         <v>45528</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <v>6.1401700000000003</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>6.1401700000000003</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="6">
         <v>6.1401700000000003</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="6">
         <f t="shared" si="0"/>
         <v>6.1401700000000003</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="6">
         <f t="shared" si="1"/>
         <v>6.1401700000000003</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="6">
         <f t="shared" si="2"/>
         <v>6.1401700000000003</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="9">
         <v>40</v>
       </c>
       <c r="B41" s="5">
         <v>45529</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>6.1401700000000003</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>6.1401700000000003</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="6">
         <v>6.1395999999999997</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="6">
         <f t="shared" si="0"/>
         <v>6.1401700000000003</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="6">
         <f t="shared" si="1"/>
         <v>6.1395999999999997</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="6">
         <f t="shared" si="2"/>
         <v>6.1399800000000004</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="9">
         <v>41</v>
       </c>
       <c r="B42" s="5">
         <v>45530</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="6">
         <v>6.1208999999999998</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="6">
         <v>6.1284999999999998</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="6">
         <v>6.1401000000000003</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="6">
         <f t="shared" si="0"/>
         <v>6.1401000000000003</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="6">
         <f t="shared" si="1"/>
         <v>6.1208999999999998</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="6">
         <f t="shared" si="2"/>
         <v>6.129833333333333</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="9">
         <v>42</v>
       </c>
       <c r="B43" s="5">
         <v>45531</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="6">
         <v>6.1345000000000001</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="6">
         <v>6.1538000000000004</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="6">
         <v>6.1562000000000001</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="6">
         <f t="shared" si="0"/>
         <v>6.1562000000000001</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="6">
         <f t="shared" si="1"/>
         <v>6.1345000000000001</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="6">
         <f t="shared" si="2"/>
         <v>6.1481666666666657</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="9">
         <v>43</v>
       </c>
       <c r="B44" s="5">
         <v>45532</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="6">
         <v>6.1444999999999999</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="6">
         <v>6.1733000000000002</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="6">
         <v>6.1912000000000003</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="6">
         <f t="shared" si="0"/>
         <v>6.1912000000000003</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="6">
         <f t="shared" si="1"/>
         <v>6.1444999999999999</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="6">
         <f t="shared" si="2"/>
         <v>6.1696666666666671</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="9">
         <v>44</v>
       </c>
       <c r="B45" s="5">
         <v>45533</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="6">
         <v>6.2511999999999999</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="6">
         <v>6.2274000000000003</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="6">
         <v>6.2314999999999996</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="6">
         <f t="shared" si="0"/>
         <v>6.2511999999999999</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="6">
         <f t="shared" si="1"/>
         <v>6.2274000000000003</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="6">
         <f t="shared" si="2"/>
         <v>6.2366999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="9">
         <v>45</v>
       </c>
       <c r="B46" s="5">
         <v>45534</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="6">
         <v>6.2614000000000001</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="6">
         <v>6.2282000000000002</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="6">
         <v>6.1933699999999998</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="6">
         <f t="shared" si="0"/>
         <v>6.2614000000000001</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="6">
         <f t="shared" si="1"/>
         <v>6.1933699999999998</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="6">
         <f t="shared" si="2"/>
         <v>6.2276566666666655</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="9">
         <v>46</v>
       </c>
       <c r="B47" s="5">
         <v>45535</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="6">
         <v>6.1933699999999998</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="6">
         <v>6.1933699999999998</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="6">
         <v>6.1933699999999998</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="6">
         <f t="shared" si="0"/>
         <v>6.1933699999999998</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="6">
         <f t="shared" si="1"/>
         <v>6.1933699999999998</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="6">
         <f t="shared" si="2"/>
         <v>6.1933699999999989</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="9">
         <v>47</v>
       </c>
       <c r="B48" s="5">
         <v>45536</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="6">
         <v>6.1933699999999998</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="6">
         <v>6.1933699999999998</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="6">
         <v>6.2034399999999996</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="6">
         <f t="shared" si="0"/>
         <v>6.2034399999999996</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="6">
         <f t="shared" si="1"/>
         <v>6.1933699999999998</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="6">
         <f t="shared" si="2"/>
         <v>6.1967266666666667</v>
       </c>

</xml_diff>

<commit_message>
another day another dollar... and euro
</commit_message>
<xml_diff>
--- a/excel/exchanges_historic_series.xlsx
+++ b/excel/exchanges_historic_series.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDC08B3-2099-4F23-B484-0B41BC4F0880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F60DA58-78FE-4A6B-AEBC-C688BC5C9EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="20">
   <si>
     <t>date</t>
   </si>
@@ -96,6 +96,9 @@
   <si>
     <t>48</t>
   </si>
+  <si>
+    <t>49</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -159,7 +162,6 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,10 +380,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143:C145"/>
+      <selection activeCell="C146" sqref="C146:C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4129,6 +4131,84 @@
         <v>11</v>
       </c>
     </row>
+    <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="5">
+        <v>45538</v>
+      </c>
+      <c r="B146">
+        <v>6.2251500000000002</v>
+      </c>
+      <c r="C146">
+        <v>5.6275700000000004</v>
+      </c>
+      <c r="D146">
+        <v>6.3532400000000004</v>
+      </c>
+      <c r="E146">
+        <v>5.7504299999999997</v>
+      </c>
+      <c r="F146">
+        <v>6.22</v>
+      </c>
+      <c r="G146">
+        <v>5.63</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="5">
+        <v>45538</v>
+      </c>
+      <c r="B147">
+        <v>6.2280600000000002</v>
+      </c>
+      <c r="C147">
+        <v>5.6402099999999997</v>
+      </c>
+      <c r="D147">
+        <v>5.6313199999999997</v>
+      </c>
+      <c r="E147">
+        <v>5.7636799999999999</v>
+      </c>
+      <c r="F147">
+        <v>6.23</v>
+      </c>
+      <c r="G147">
+        <v>5.65</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="5">
+        <v>45538</v>
+      </c>
+      <c r="B148">
+        <v>6.2437500000000004</v>
+      </c>
+      <c r="C148">
+        <v>5.6492100000000001</v>
+      </c>
+      <c r="D148">
+        <v>6.3491999999999997</v>
+      </c>
+      <c r="E148">
+        <v>5.7636799999999999</v>
+      </c>
+      <c r="F148">
+        <v>6.24</v>
+      </c>
+      <c r="G148">
+        <v>5.65</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4136,16 +4216,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47E47A6-69F4-4AEB-9879-64F1134C7037}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="6"/>
     <col min="4" max="4" width="11.5703125" style="6" customWidth="1"/>
     <col min="5" max="8" width="9.140625" style="6"/>
@@ -5544,7 +5624,7 @@
       <c r="A49" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="5">
         <v>45537</v>
       </c>
       <c r="C49">
@@ -5567,6 +5647,35 @@
       <c r="H49" s="6">
         <f t="shared" si="2"/>
         <v>5.6309866666666659</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="5">
+        <v>45538</v>
+      </c>
+      <c r="C50">
+        <v>5.6275700000000004</v>
+      </c>
+      <c r="D50">
+        <v>5.6402099999999997</v>
+      </c>
+      <c r="E50">
+        <v>5.6492100000000001</v>
+      </c>
+      <c r="F50" s="6">
+        <f t="shared" ref="F50" si="3">LARGE(C50:E50,1)</f>
+        <v>5.6492100000000001</v>
+      </c>
+      <c r="G50" s="6">
+        <f t="shared" ref="G50" si="4">SMALL(C50:E50,1)</f>
+        <v>5.6275700000000004</v>
+      </c>
+      <c r="H50" s="6">
+        <f t="shared" ref="H50" si="5">AVERAGE(C50:E50)</f>
+        <v>5.6389966666666664</v>
       </c>
     </row>
   </sheetData>
@@ -5582,7 +5691,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7013,9 +7122,38 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="5"/>
+      <c r="A50" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="5">
+        <v>45538</v>
+      </c>
+      <c r="C50">
+        <v>6.2251500000000002</v>
+      </c>
+      <c r="D50">
+        <v>6.2280600000000002</v>
+      </c>
+      <c r="E50">
+        <v>6.2437500000000004</v>
+      </c>
+      <c r="F50" s="6">
+        <f t="shared" ref="F50" si="3">LARGE(C50:E50,1)</f>
+        <v>6.2437500000000004</v>
+      </c>
+      <c r="G50" s="6">
+        <f t="shared" ref="G50" si="4">SMALL(C50:E50,1)</f>
+        <v>6.2251500000000002</v>
+      </c>
+      <c r="H50" s="6">
+        <f t="shared" ref="H50" si="5">AVERAGE(C50:E50)</f>
+        <v>6.2323200000000005</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError sqref="A49:A50" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
another day, another... euro?
</commit_message>
<xml_diff>
--- a/excel/exchanges_historic_series.xlsx
+++ b/excel/exchanges_historic_series.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F60DA58-78FE-4A6B-AEBC-C688BC5C9EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6172DA-0D97-46E8-9214-BA7F1297D932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="21">
   <si>
     <t>date</t>
   </si>
@@ -99,6 +99,9 @@
   <si>
     <t>49</t>
   </si>
+  <si>
+    <t>50</t>
+  </si>
 </sst>
 </file>
 
@@ -151,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -162,6 +165,7 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,10 +384,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146:C148"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149:C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4209,6 +4213,84 @@
         <v>11</v>
       </c>
     </row>
+    <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="5">
+        <v>45539</v>
+      </c>
+      <c r="B149">
+        <v>6.2382799999999996</v>
+      </c>
+      <c r="C149">
+        <v>5.6345700000000001</v>
+      </c>
+      <c r="D149">
+        <v>6.3572699999999998</v>
+      </c>
+      <c r="E149">
+        <v>5.7306499999999998</v>
+      </c>
+      <c r="F149">
+        <v>6.23</v>
+      </c>
+      <c r="G149">
+        <v>5.62</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="5">
+        <v>45539</v>
+      </c>
+      <c r="B150">
+        <v>6.2497699999999998</v>
+      </c>
+      <c r="C150">
+        <v>5.6393000000000004</v>
+      </c>
+      <c r="D150">
+        <v>6.3856900000000003</v>
+      </c>
+      <c r="E150">
+        <v>5.75373</v>
+      </c>
+      <c r="F150">
+        <v>6.24</v>
+      </c>
+      <c r="G150">
+        <v>5.64</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="5">
+        <v>45539</v>
+      </c>
+      <c r="B151">
+        <v>6.2532800000000002</v>
+      </c>
+      <c r="C151">
+        <v>5.6435000000000004</v>
+      </c>
+      <c r="D151">
+        <v>6.3856900000000003</v>
+      </c>
+      <c r="E151">
+        <v>5.7570499999999996</v>
+      </c>
+      <c r="F151">
+        <v>6.24</v>
+      </c>
+      <c r="G151">
+        <v>5.64</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4216,10 +4298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47E47A6-69F4-4AEB-9879-64F1134C7037}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5678,6 +5760,35 @@
         <v>5.6389966666666664</v>
       </c>
     </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="5">
+        <v>45539</v>
+      </c>
+      <c r="C51">
+        <v>5.6345700000000001</v>
+      </c>
+      <c r="D51">
+        <v>5.6393000000000004</v>
+      </c>
+      <c r="E51">
+        <v>5.6435000000000004</v>
+      </c>
+      <c r="F51" s="6">
+        <f t="shared" ref="F51" si="6">LARGE(C51:E51,1)</f>
+        <v>5.6435000000000004</v>
+      </c>
+      <c r="G51" s="6">
+        <f t="shared" ref="G51" si="7">SMALL(C51:E51,1)</f>
+        <v>5.6345700000000001</v>
+      </c>
+      <c r="H51" s="6">
+        <f t="shared" ref="H51" si="8">AVERAGE(C51:E51)</f>
+        <v>5.6391233333333339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
@@ -5688,10 +5799,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599224F4-1114-46B0-AF99-277C0227B676}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7150,6 +7261,35 @@
         <v>6.2323200000000005</v>
       </c>
     </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="10">
+        <v>45539</v>
+      </c>
+      <c r="C51">
+        <v>6.2382799999999996</v>
+      </c>
+      <c r="D51">
+        <v>6.2497699999999998</v>
+      </c>
+      <c r="E51">
+        <v>6.2532800000000002</v>
+      </c>
+      <c r="F51" s="6">
+        <f t="shared" ref="F51" si="6">LARGE(C51:E51,1)</f>
+        <v>6.2532800000000002</v>
+      </c>
+      <c r="G51" s="6">
+        <f t="shared" ref="G51" si="7">SMALL(C51:E51,1)</f>
+        <v>6.2382799999999996</v>
+      </c>
+      <c r="H51" s="6">
+        <f t="shared" ref="H51" si="8">AVERAGE(C51:E51)</f>
+        <v>6.2471099999999993</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
adds arima specific datasets
</commit_message>
<xml_diff>
--- a/excel/exchanges_historic_series.xlsx
+++ b/excel/exchanges_historic_series.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\Documents\Programming\MBA\xchange\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2EA117-1BD6-4604-B988-4BCFEFE0153A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FD79CF-93B8-4B88-AE85-7045A55DC667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="1" r:id="rId1"/>
     <sheet name="2024_wise_usd" sheetId="2" r:id="rId2"/>
-    <sheet name="2024_wise_eur" sheetId="3" r:id="rId3"/>
-    <sheet name="2024_wise_desc" sheetId="4" r:id="rId4"/>
+    <sheet name="2024_usd_arima" sheetId="5" r:id="rId3"/>
+    <sheet name="2024_wise_eur" sheetId="3" r:id="rId4"/>
+    <sheet name="2024_eur_arima" sheetId="6" r:id="rId5"/>
+    <sheet name="2024_wise_desc" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2024_wise_eur'!$B$1:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2024_wise_eur'!$B$1:$F$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -189,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="65">
   <si>
     <t>date</t>
   </si>
@@ -308,9 +310,6 @@
     <t>retornoDiscreto</t>
   </si>
   <si>
-    <t>retornoContínuo</t>
-  </si>
-  <si>
     <t>Retorno Contínuo Médio</t>
   </si>
   <si>
@@ -382,12 +381,18 @@
   <si>
     <t>61</t>
   </si>
+  <si>
+    <t>retornoContinuo</t>
+  </si>
+  <si>
+    <t>dayTime</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
@@ -398,6 +403,7 @@
     <numFmt numFmtId="171" formatCode="0.0000"/>
     <numFmt numFmtId="172" formatCode="0.0000000"/>
     <numFmt numFmtId="173" formatCode="0.00000000"/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd\ hh:mm:ss\.&quot;000&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -476,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -501,6 +507,7 @@
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,8 +730,8 @@
   <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D179" sqref="D179:D181"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6678,7 +6685,7 @@
     </row>
     <row r="182" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F182" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -6691,8 +6698,8 @@
   <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6743,7 +6750,7 @@
         <v>38</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>37</v>
@@ -9734,7 +9741,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="5">
         <v>45544</v>
@@ -9790,7 +9797,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="5">
         <v>45545</v>
@@ -9846,7 +9853,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="5">
         <v>45546</v>
@@ -9902,7 +9909,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="5">
         <v>45547</v>
@@ -9958,7 +9965,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="5">
         <v>45548</v>
@@ -10014,7 +10021,7 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" s="5">
         <v>45549</v>
@@ -10070,7 +10077,7 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="5">
         <v>45550</v>
@@ -10127,12 +10134,1479 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48303F0D-A187-4586-8FC5-1A0B7B975EA0}">
+  <dimension ref="A1:B181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="24">
+        <v>45490.458333333336</v>
+      </c>
+      <c r="B2">
+        <v>5.4586899999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="24">
+        <v>45490.708333333336</v>
+      </c>
+      <c r="B3">
+        <v>5.4864600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
+        <v>45490.958333333336</v>
+      </c>
+      <c r="B4">
+        <v>5.4898899999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>45491.458333333336</v>
+      </c>
+      <c r="B5">
+        <v>5.4920900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
+        <v>45491.708333333336</v>
+      </c>
+      <c r="B6">
+        <v>5.5887500000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="24">
+        <v>45491.958333333336</v>
+      </c>
+      <c r="B7">
+        <v>5.5447100000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="24">
+        <v>45492.458333333336</v>
+      </c>
+      <c r="B8">
+        <v>5.5445000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="24">
+        <v>45492.708333333336</v>
+      </c>
+      <c r="B9">
+        <v>5.5788599999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="24">
+        <v>45492.958333333336</v>
+      </c>
+      <c r="B10">
+        <v>5.59816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="24">
+        <v>45493.458333333336</v>
+      </c>
+      <c r="B11">
+        <v>5.59816</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
+        <v>45493.708333333336</v>
+      </c>
+      <c r="B12">
+        <v>5.59816</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="24">
+        <v>45493.958333333336</v>
+      </c>
+      <c r="B13">
+        <v>5.59816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="24">
+        <v>45494.458333333336</v>
+      </c>
+      <c r="B14">
+        <v>5.59816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="24">
+        <v>45494.458333333336</v>
+      </c>
+      <c r="B15">
+        <v>5.59816</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="24">
+        <v>45494.708333333336</v>
+      </c>
+      <c r="B16">
+        <v>5.5453000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="24">
+        <v>45495.958333333336</v>
+      </c>
+      <c r="B17">
+        <v>5.5717100000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="24">
+        <v>45495.458333333336</v>
+      </c>
+      <c r="B18">
+        <v>5.5692599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="24">
+        <v>45495.708333333336</v>
+      </c>
+      <c r="B19">
+        <v>5.5720900000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="24">
+        <v>45496.958333333336</v>
+      </c>
+      <c r="B20">
+        <v>5.5933099999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="24">
+        <v>45496.458333333336</v>
+      </c>
+      <c r="B21">
+        <v>5.5861900000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="24">
+        <v>45496.708333333336</v>
+      </c>
+      <c r="B22">
+        <v>5.5865600000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="24">
+        <v>45497.958333333336</v>
+      </c>
+      <c r="B23">
+        <v>5.6412399999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="24">
+        <v>45497.458333333336</v>
+      </c>
+      <c r="B24">
+        <v>5.6542899999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="24">
+        <v>45497.708333333336</v>
+      </c>
+      <c r="B25">
+        <v>5.6550500000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="24">
+        <v>45498.958333333336</v>
+      </c>
+      <c r="B26">
+        <v>5.6501999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="24">
+        <v>45498.458333333336</v>
+      </c>
+      <c r="B27">
+        <v>5.64764</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="24">
+        <v>45498.458333333336</v>
+      </c>
+      <c r="B28">
+        <v>5.6452499999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="24">
+        <v>45499.708333333336</v>
+      </c>
+      <c r="B29">
+        <v>5.6402900000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="24">
+        <v>45499.958333333336</v>
+      </c>
+      <c r="B30">
+        <v>5.6578400000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="24">
+        <v>45499.458333333336</v>
+      </c>
+      <c r="B31">
+        <v>5.6562999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="24">
+        <v>45500.708333333336</v>
+      </c>
+      <c r="B32">
+        <v>5.6562999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="24">
+        <v>45500.958333333336</v>
+      </c>
+      <c r="B33">
+        <v>5.6562999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="24">
+        <v>45500.458333333336</v>
+      </c>
+      <c r="B34">
+        <v>5.6562999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="24">
+        <v>45501.708333333336</v>
+      </c>
+      <c r="B35">
+        <v>5.6562999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="24">
+        <v>45501.958333333336</v>
+      </c>
+      <c r="B36">
+        <v>5.65665</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="24">
+        <v>45501.458333333336</v>
+      </c>
+      <c r="B37">
+        <v>5.6568100000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="24">
+        <v>45502.708333333336</v>
+      </c>
+      <c r="B38">
+        <v>5.6509</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="24">
+        <v>45502.958333333336</v>
+      </c>
+      <c r="B39">
+        <v>5.6242999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="24">
+        <v>45502.458333333336</v>
+      </c>
+      <c r="B40">
+        <v>5.6160800000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="24">
+        <v>45503.708333333336</v>
+      </c>
+      <c r="B41">
+        <v>5.6556600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="24">
+        <v>45503.958333333336</v>
+      </c>
+      <c r="B42">
+        <v>5.6123000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="24">
+        <v>45503.458333333336</v>
+      </c>
+      <c r="B43">
+        <v>5.6125499999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="24">
+        <v>45504.458333333336</v>
+      </c>
+      <c r="B44">
+        <v>5.6746600000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="24">
+        <v>45504.708333333336</v>
+      </c>
+      <c r="B45">
+        <v>5.6479900000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="24">
+        <v>45504.958333333336</v>
+      </c>
+      <c r="B46">
+        <v>5.6578999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="24">
+        <v>45505.458333333336</v>
+      </c>
+      <c r="B47">
+        <v>5.6421900000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="24">
+        <v>45505.708333333336</v>
+      </c>
+      <c r="B48">
+        <v>5.7348699999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="24">
+        <v>45505.958333333336</v>
+      </c>
+      <c r="B49">
+        <v>5.7524199999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="24">
+        <v>45506.458333333336</v>
+      </c>
+      <c r="B50">
+        <v>5.7158499999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="24">
+        <v>45506.708333333336</v>
+      </c>
+      <c r="B51">
+        <v>5.7095900000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="24">
+        <v>45506.958333333336</v>
+      </c>
+      <c r="B52">
+        <v>5.7280699999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="24">
+        <v>45507.458333333336</v>
+      </c>
+      <c r="B53">
+        <v>5.7280699999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="24">
+        <v>45507.458333333336</v>
+      </c>
+      <c r="B54">
+        <v>5.7280699999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="24">
+        <v>45507.708333333336</v>
+      </c>
+      <c r="B55">
+        <v>5.7280699999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="24">
+        <v>45508.958333333336</v>
+      </c>
+      <c r="B56">
+        <v>5.7280699999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="24">
+        <v>45508.458333333336</v>
+      </c>
+      <c r="B57">
+        <v>5.7272100000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="24">
+        <v>45508.708333333336</v>
+      </c>
+      <c r="B58">
+        <v>5.7281000000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="24">
+        <v>45509.958333333336</v>
+      </c>
+      <c r="B59">
+        <v>5.8010999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="24">
+        <v>45509.458333333336</v>
+      </c>
+      <c r="B60">
+        <v>5.7407599999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="24">
+        <v>45509.708333333336</v>
+      </c>
+      <c r="B61">
+        <v>5.7229799999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="24">
+        <v>45510.958333333336</v>
+      </c>
+      <c r="B62">
+        <v>5.6627099999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="24">
+        <v>45510.458333333336</v>
+      </c>
+      <c r="B63">
+        <v>5.6586100000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="24">
+        <v>45510.708333333336</v>
+      </c>
+      <c r="B64">
+        <v>5.6571600000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="24">
+        <v>45511.958333333336</v>
+      </c>
+      <c r="B65">
+        <v>5.6033099999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="24">
+        <v>45511.458333333336</v>
+      </c>
+      <c r="B66">
+        <v>5.6236600000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="24">
+        <v>45511.458333333336</v>
+      </c>
+      <c r="B67">
+        <v>5.6373899999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="24">
+        <v>45512.708333333336</v>
+      </c>
+      <c r="B68">
+        <v>5.617</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="24">
+        <v>45512.958333333336</v>
+      </c>
+      <c r="B69">
+        <v>5.5742599999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="24">
+        <v>45512.458333333336</v>
+      </c>
+      <c r="B70">
+        <v>5.5475099999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="24">
+        <v>45513.458333333336</v>
+      </c>
+      <c r="B71">
+        <v>5.5172400000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="24">
+        <v>45513.708333333336</v>
+      </c>
+      <c r="B72">
+        <v>5.5146600000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="24">
+        <v>45513.958333333336</v>
+      </c>
+      <c r="B73">
+        <v>5.5087000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="24">
+        <v>45514.458333333336</v>
+      </c>
+      <c r="B74">
+        <v>5.5087000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="24">
+        <v>45514.708333333336</v>
+      </c>
+      <c r="B75">
+        <v>5.5087000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="24">
+        <v>45514.958333333336</v>
+      </c>
+      <c r="B76">
+        <v>5.5087000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="24">
+        <v>45515.458333333336</v>
+      </c>
+      <c r="B77">
+        <v>5.4993999999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="24">
+        <v>45515.708333333336</v>
+      </c>
+      <c r="B78">
+        <v>5.4977400000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="24">
+        <v>45515.958333333336</v>
+      </c>
+      <c r="B79">
+        <v>5.4938399999999996</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="24">
+        <v>45516.458333333336</v>
+      </c>
+      <c r="B80">
+        <v>5.4993999999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="24">
+        <v>45516.708333333336</v>
+      </c>
+      <c r="B81">
+        <v>5.4877399999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="24">
+        <v>45516.958333333336</v>
+      </c>
+      <c r="B82">
+        <v>5.4938399999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="24">
+        <v>45517.458333333336</v>
+      </c>
+      <c r="B83">
+        <v>5.4891100000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="24">
+        <v>45517.458333333336</v>
+      </c>
+      <c r="B84">
+        <v>5.4487899999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="24">
+        <v>45517.708333333336</v>
+      </c>
+      <c r="B85">
+        <v>5.4572900000000004</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="24">
+        <v>45518.958333333336</v>
+      </c>
+      <c r="B86">
+        <v>5.44909</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="24">
+        <v>45518.458333333336</v>
+      </c>
+      <c r="B87">
+        <v>5.46896</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="24">
+        <v>45518.458333333336</v>
+      </c>
+      <c r="B88">
+        <v>5.4706099999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="24">
+        <v>45519.708333333336</v>
+      </c>
+      <c r="B89">
+        <v>5.4555100000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="24">
+        <v>45519.958333333336</v>
+      </c>
+      <c r="B90">
+        <v>5.4836900000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="24">
+        <v>45519.458333333336</v>
+      </c>
+      <c r="B91">
+        <v>5.4863400000000002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="24">
+        <v>45520.708333333336</v>
+      </c>
+      <c r="B92">
+        <v>5.4542599999999997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="24">
+        <v>45520.958333333336</v>
+      </c>
+      <c r="B93">
+        <v>5.46624</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="24">
+        <v>45520.458333333336</v>
+      </c>
+      <c r="B94">
+        <v>5.4715400000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="24">
+        <v>45521.708333333336</v>
+      </c>
+      <c r="B95">
+        <v>5.4715400000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="24">
+        <v>45521.958333333336</v>
+      </c>
+      <c r="B96">
+        <v>5.4715400000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="24">
+        <v>45521.458333333336</v>
+      </c>
+      <c r="B97">
+        <v>5.4715400000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="24">
+        <v>45522.708333333336</v>
+      </c>
+      <c r="B98">
+        <v>5.4715400000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="24">
+        <v>45522.958333333336</v>
+      </c>
+      <c r="B99">
+        <v>5.4715400000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="24">
+        <v>45522.458333333336</v>
+      </c>
+      <c r="B100">
+        <v>5.4694000000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="24">
+        <v>45523.458333333336</v>
+      </c>
+      <c r="B101">
+        <v>5.4292999999999996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="24">
+        <v>45523.708333333336</v>
+      </c>
+      <c r="B102">
+        <v>5.4124999999999996</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="24">
+        <v>45523.958333333336</v>
+      </c>
+      <c r="B103">
+        <v>5.4063999999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="24">
+        <v>45524.458333333336</v>
+      </c>
+      <c r="B104">
+        <v>5.4397000000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="24">
+        <v>45524.708333333336</v>
+      </c>
+      <c r="B105">
+        <v>5.4852999999999996</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="24">
+        <v>45524.958333333336</v>
+      </c>
+      <c r="B106">
+        <v>5.4795999999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="24">
+        <v>45525.458333333336</v>
+      </c>
+      <c r="B107">
+        <v>5.47</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="24">
+        <v>45525.708333333336</v>
+      </c>
+      <c r="B108">
+        <v>5.4812000000000003</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="24">
+        <v>45525.958333333336</v>
+      </c>
+      <c r="B109">
+        <v>5.4836999999999998</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="24">
+        <v>45526.458333333336</v>
+      </c>
+      <c r="B110">
+        <v>5.5452000000000004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="24">
+        <v>45526.708333333336</v>
+      </c>
+      <c r="B111">
+        <v>5.5896999999999997</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="24">
+        <v>45526.958333333336</v>
+      </c>
+      <c r="B112">
+        <v>5.5921000000000003</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="24">
+        <v>45527.458333333336</v>
+      </c>
+      <c r="B113">
+        <v>5.5518000000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="24">
+        <v>45527.708333333336</v>
+      </c>
+      <c r="B114">
+        <v>5.4794999999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="24">
+        <v>45527.958333333336</v>
+      </c>
+      <c r="B115">
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="24">
+        <v>45528.458333333336</v>
+      </c>
+      <c r="B116">
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="24">
+        <v>45528.458333333336</v>
+      </c>
+      <c r="B117">
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="24">
+        <v>45528.708333333336</v>
+      </c>
+      <c r="B118">
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="24">
+        <v>45529.958333333336</v>
+      </c>
+      <c r="B119">
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="24">
+        <v>45529.458333333336</v>
+      </c>
+      <c r="B120">
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="24">
+        <v>45529.708333333336</v>
+      </c>
+      <c r="B121">
+        <v>5.4859499999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="24">
+        <v>45530.458333333336</v>
+      </c>
+      <c r="B122">
+        <v>5.4848999999999997</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="24">
+        <v>45530.708333333336</v>
+      </c>
+      <c r="B123">
+        <v>5.4917999999999996</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="24">
+        <v>45530.958333333336</v>
+      </c>
+      <c r="B124">
+        <v>5.4972000000000003</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="24">
+        <v>45531.458333333336</v>
+      </c>
+      <c r="B125">
+        <v>5.4927000000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="24">
+        <v>45531.708333333336</v>
+      </c>
+      <c r="B126">
+        <v>5.5025000000000004</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="24">
+        <v>45531.958333333336</v>
+      </c>
+      <c r="B127">
+        <v>5.5094000000000003</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="24">
+        <v>45532.458333333336</v>
+      </c>
+      <c r="B128">
+        <v>5.5304000000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="24">
+        <v>45532.708333333336</v>
+      </c>
+      <c r="B129">
+        <v>5.5549799999999996</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="24">
+        <v>45532.958333333336</v>
+      </c>
+      <c r="B130">
+        <v>5.5633999999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="24">
+        <v>45533.458333333336</v>
+      </c>
+      <c r="B131">
+        <v>5.6406000000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="24">
+        <v>45533.708333333336</v>
+      </c>
+      <c r="B132">
+        <v>5.6227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="24">
+        <v>45533.958333333336</v>
+      </c>
+      <c r="B133">
+        <v>5.6288999999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="24">
+        <v>45534.458333333336</v>
+      </c>
+      <c r="B134">
+        <v>5.6656000000000004</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="24">
+        <v>45534.708333333336</v>
+      </c>
+      <c r="B135">
+        <v>5.6341000000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="24">
+        <v>45534.958333333336</v>
+      </c>
+      <c r="B136">
+        <v>5.6063799999999997</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="24">
+        <v>45535.458333333336</v>
+      </c>
+      <c r="B137">
+        <v>5.6063799999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="24">
+        <v>45535.708333333336</v>
+      </c>
+      <c r="B138">
+        <v>5.6063799999999997</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="24">
+        <v>45535.958333333336</v>
+      </c>
+      <c r="B139">
+        <v>5.6063799999999997</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="24">
+        <v>45536.458333333336</v>
+      </c>
+      <c r="B140">
+        <v>5.6063799999999997</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="24">
+        <v>45536.708333333336</v>
+      </c>
+      <c r="B141">
+        <v>5.6063799999999997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="24">
+        <v>45536.958333333336</v>
+      </c>
+      <c r="B142">
+        <v>5.6116900000000003</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="24">
+        <v>45537.458333333336</v>
+      </c>
+      <c r="B143">
+        <v>5.6504500000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="24">
+        <v>45537.708333333336</v>
+      </c>
+      <c r="B144">
+        <v>5.6259499999999996</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="24">
+        <v>45537.958333333336</v>
+      </c>
+      <c r="B145">
+        <v>5.6165599999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="24">
+        <v>45538.458333333336</v>
+      </c>
+      <c r="B146">
+        <v>5.6275700000000004</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="24">
+        <v>45538.708333333336</v>
+      </c>
+      <c r="B147">
+        <v>5.6402099999999997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="24">
+        <v>45538.958333333336</v>
+      </c>
+      <c r="B148">
+        <v>5.6492100000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="24">
+        <v>45539.458333333336</v>
+      </c>
+      <c r="B149">
+        <v>5.6345700000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="24">
+        <v>45539.708333333336</v>
+      </c>
+      <c r="B150">
+        <v>5.6393000000000004</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="24">
+        <v>45539.958333333336</v>
+      </c>
+      <c r="B151">
+        <v>5.6435000000000004</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="24">
+        <v>45540.458333333336</v>
+      </c>
+      <c r="B152">
+        <v>5.6099100000000002</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="24">
+        <v>45540.708333333336</v>
+      </c>
+      <c r="B153">
+        <v>5.5724999999999998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="24">
+        <v>45540.958333333336</v>
+      </c>
+      <c r="B154">
+        <v>5.5689000000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="24">
+        <v>45541.458333333336</v>
+      </c>
+      <c r="B155">
+        <v>5.5615600000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="24">
+        <v>45541.708333333336</v>
+      </c>
+      <c r="B156">
+        <v>5.5899900000000002</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="24">
+        <v>45541.958333333336</v>
+      </c>
+      <c r="B157">
+        <v>5.5993899999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="24">
+        <v>45542.458333333336</v>
+      </c>
+      <c r="B158">
+        <v>5.5993899999999996</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="24">
+        <v>45542.708333333336</v>
+      </c>
+      <c r="B159">
+        <v>5.5993899999999996</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="24">
+        <v>45542.958333333336</v>
+      </c>
+      <c r="B160">
+        <v>5.5993899999999996</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="24">
+        <v>45543.458333333336</v>
+      </c>
+      <c r="B161">
+        <v>5.5993899999999996</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="24">
+        <v>45543.708333333336</v>
+      </c>
+      <c r="B162">
+        <v>5.5993899999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="24">
+        <v>45543.958333333336</v>
+      </c>
+      <c r="B163">
+        <v>5.5987099999999996</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="24">
+        <v>45544.458333333336</v>
+      </c>
+      <c r="B164">
+        <v>5.6100399999999997</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="24">
+        <v>45544.708333333336</v>
+      </c>
+      <c r="B165">
+        <v>5.5858100000000004</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="24">
+        <v>45544.958333333336</v>
+      </c>
+      <c r="B166">
+        <v>5.5851600000000001</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="24">
+        <v>45545.458333333336</v>
+      </c>
+      <c r="B167">
+        <v>5.6162900000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="24">
+        <v>45545.708333333336</v>
+      </c>
+      <c r="B168">
+        <v>5.6537199999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="24">
+        <v>45545.958333333336</v>
+      </c>
+      <c r="B169">
+        <v>5.6643100000000004</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="24">
+        <v>45546.458333333336</v>
+      </c>
+      <c r="B170">
+        <v>5.6434600000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="24">
+        <v>45546.708333333336</v>
+      </c>
+      <c r="B171">
+        <v>5.6589900000000002</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="24">
+        <v>45546.958333333336</v>
+      </c>
+      <c r="B172">
+        <v>5.66906</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="24">
+        <v>45547.458333333336</v>
+      </c>
+      <c r="B173">
+        <v>5.6587300000000003</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="24">
+        <v>45547.708333333336</v>
+      </c>
+      <c r="B174">
+        <v>5.6176599999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="24">
+        <v>45547.958333333336</v>
+      </c>
+      <c r="B175">
+        <v>5.6271199999999997</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="24">
+        <v>45548.458333333336</v>
+      </c>
+      <c r="B176">
+        <v>5.5726899999999997</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="24">
+        <v>45548.708333333336</v>
+      </c>
+      <c r="B177">
+        <v>5.5674000000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="24">
+        <v>45548.958333333336</v>
+      </c>
+      <c r="B178">
+        <v>5.5648</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="24">
+        <v>45549.458333333336</v>
+      </c>
+      <c r="B179">
+        <v>5.5648</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="24">
+        <v>45549.708333333336</v>
+      </c>
+      <c r="B180">
+        <v>5.5648</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="24">
+        <v>45549.958333333336</v>
+      </c>
+      <c r="B181">
+        <v>5.5648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599224F4-1114-46B0-AF99-277C0227B676}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10182,7 +11656,7 @@
         <v>38</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>37</v>
@@ -13173,7 +14647,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="5">
         <v>45544</v>
@@ -13229,7 +14703,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="5">
         <v>45545</v>
@@ -13285,7 +14759,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="5">
         <v>45546</v>
@@ -13341,7 +14815,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="5">
         <v>45547</v>
@@ -13397,7 +14871,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="5">
         <v>45548</v>
@@ -13453,7 +14927,7 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" s="5">
         <v>45549</v>
@@ -13509,7 +14983,7 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="5">
         <v>45550</v>
@@ -13580,7 +15054,1473 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68288BB6-1299-407F-A20E-500DE3875D7F}">
+  <dimension ref="A1:B181"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" style="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="24">
+        <v>45490.458333333336</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5.9731800000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="24">
+        <v>45490.708333333336</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5.9967499999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
+        <v>45490.958333333336</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6.0023600000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>45491.458333333336</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6.00298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
+        <v>45491.708333333336</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6.0900600000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="24">
+        <v>45491.958333333336</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6.0370799999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="24">
+        <v>45492.458333333336</v>
+      </c>
+      <c r="B8" s="18">
+        <v>6.0396299999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="24">
+        <v>45492.708333333336</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6.0720099999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="24">
+        <v>45492.958333333336</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6.0924699999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="24">
+        <v>45493.458333333336</v>
+      </c>
+      <c r="B11">
+        <v>6.0924699999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
+        <v>45493.708333333336</v>
+      </c>
+      <c r="B12">
+        <v>6.0924699999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="24">
+        <v>45493.958333333336</v>
+      </c>
+      <c r="B13">
+        <v>6.0924699999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="24">
+        <v>45494.458333333336</v>
+      </c>
+      <c r="B14">
+        <v>6.0924699999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="24">
+        <v>45494.458333333336</v>
+      </c>
+      <c r="B15">
+        <v>6.0924699999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="24">
+        <v>45494.708333333336</v>
+      </c>
+      <c r="B16">
+        <v>6.0363499999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="24">
+        <v>45495.958333333336</v>
+      </c>
+      <c r="B17">
+        <v>6.0609000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="24">
+        <v>45495.458333333336</v>
+      </c>
+      <c r="B18">
+        <v>6.06351</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="24">
+        <v>45495.708333333336</v>
+      </c>
+      <c r="B19">
+        <v>6.0671900000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="24">
+        <v>45496.958333333336</v>
+      </c>
+      <c r="B20">
+        <v>6.0692899999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="24">
+        <v>45496.458333333336</v>
+      </c>
+      <c r="B21">
+        <v>6.0613000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="24">
+        <v>45496.708333333336</v>
+      </c>
+      <c r="B22">
+        <v>6.0602799999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="24">
+        <v>45497.958333333336</v>
+      </c>
+      <c r="B23">
+        <v>6.1232899999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="24">
+        <v>45497.458333333336</v>
+      </c>
+      <c r="B24">
+        <v>6.1300400000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="24">
+        <v>45497.708333333336</v>
+      </c>
+      <c r="B25">
+        <v>6.1289499999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="24">
+        <v>45498.958333333336</v>
+      </c>
+      <c r="B26">
+        <v>6.1245200000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="24">
+        <v>45498.458333333336</v>
+      </c>
+      <c r="B27">
+        <v>6.1251600000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="24">
+        <v>45498.458333333336</v>
+      </c>
+      <c r="B28">
+        <v>6.1287700000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="24">
+        <v>45499.708333333336</v>
+      </c>
+      <c r="B29">
+        <v>6.1281999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="24">
+        <v>45499.958333333336</v>
+      </c>
+      <c r="B30">
+        <v>6.1429999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="24">
+        <v>45499.458333333336</v>
+      </c>
+      <c r="B31">
+        <v>6.1404699999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="24">
+        <v>45500.708333333336</v>
+      </c>
+      <c r="B32">
+        <v>6.1404699999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="24">
+        <v>45500.958333333336</v>
+      </c>
+      <c r="B33">
+        <v>6.1404699999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="24">
+        <v>45500.458333333336</v>
+      </c>
+      <c r="B34">
+        <v>6.1404699999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="24">
+        <v>45501.708333333336</v>
+      </c>
+      <c r="B35">
+        <v>6.1404699999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="24">
+        <v>45501.958333333336</v>
+      </c>
+      <c r="B36">
+        <v>6.1428500000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="24">
+        <v>45501.458333333336</v>
+      </c>
+      <c r="B37">
+        <v>6.1418600000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="24">
+        <v>45502.708333333336</v>
+      </c>
+      <c r="B38">
+        <v>6.1089200000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="24">
+        <v>45502.958333333336</v>
+      </c>
+      <c r="B39">
+        <v>6.08887</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="24">
+        <v>45502.458333333336</v>
+      </c>
+      <c r="B40">
+        <v>6.0749300000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="24">
+        <v>45503.708333333336</v>
+      </c>
+      <c r="B41">
+        <v>6.1143400000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="24">
+        <v>45503.958333333336</v>
+      </c>
+      <c r="B42">
+        <v>6.0705400000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="24">
+        <v>45503.458333333336</v>
+      </c>
+      <c r="B43">
+        <v>6.0747400000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="24">
+        <v>45504.458333333336</v>
+      </c>
+      <c r="B44">
+        <v>6.15245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="24">
+        <v>45504.708333333336</v>
+      </c>
+      <c r="B45">
+        <v>6.1144100000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="24">
+        <v>45504.958333333336</v>
+      </c>
+      <c r="B46">
+        <v>6.1261000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="24">
+        <v>45505.458333333336</v>
+      </c>
+      <c r="B47">
+        <v>6.0955500000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="24">
+        <v>45505.708333333336</v>
+      </c>
+      <c r="B48">
+        <v>6.1876199999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="24">
+        <v>45505.958333333336</v>
+      </c>
+      <c r="B49">
+        <v>6.2071300000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="24">
+        <v>45506.458333333336</v>
+      </c>
+      <c r="B50">
+        <v>6.2333999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="24">
+        <v>45506.708333333336</v>
+      </c>
+      <c r="B51">
+        <v>6.23088</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="24">
+        <v>45506.958333333336</v>
+      </c>
+      <c r="B52">
+        <v>6.2495700000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="24">
+        <v>45507.458333333336</v>
+      </c>
+      <c r="B53">
+        <v>6.2495700000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="24">
+        <v>45507.458333333336</v>
+      </c>
+      <c r="B54">
+        <v>6.2495700000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="24">
+        <v>45507.708333333336</v>
+      </c>
+      <c r="B55">
+        <v>6.2495700000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="24">
+        <v>45508.958333333336</v>
+      </c>
+      <c r="B56">
+        <v>6.2495700000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="24">
+        <v>45508.458333333336</v>
+      </c>
+      <c r="B57">
+        <v>6.2564099999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="24">
+        <v>45508.708333333336</v>
+      </c>
+      <c r="B58">
+        <v>6.25481</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="24">
+        <v>45509.958333333336</v>
+      </c>
+      <c r="B59">
+        <v>6.3701999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="24">
+        <v>45509.458333333336</v>
+      </c>
+      <c r="B60">
+        <v>6.2915599999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="24">
+        <v>45509.708333333336</v>
+      </c>
+      <c r="B61">
+        <v>6.2695499999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="24">
+        <v>45510.958333333336</v>
+      </c>
+      <c r="B62">
+        <v>6.1828000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="24">
+        <v>45510.458333333336</v>
+      </c>
+      <c r="B63">
+        <v>6.1848700000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="24">
+        <v>45510.708333333336</v>
+      </c>
+      <c r="B64">
+        <v>6.1767700000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="24">
+        <v>45511.958333333336</v>
+      </c>
+      <c r="B65">
+        <v>6.1179699999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="24">
+        <v>45511.458333333336</v>
+      </c>
+      <c r="B66">
+        <v>6.1429999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="24">
+        <v>45511.458333333336</v>
+      </c>
+      <c r="B67">
+        <v>6.1602499999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="24">
+        <v>45512.708333333336</v>
+      </c>
+      <c r="B68">
+        <v>6.1177400000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="24">
+        <v>45512.958333333336</v>
+      </c>
+      <c r="B69">
+        <v>6.0851300000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="24">
+        <v>45512.458333333336</v>
+      </c>
+      <c r="B70">
+        <v>6.0570500000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="24">
+        <v>45513.458333333336</v>
+      </c>
+      <c r="B71">
+        <v>6.0171000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="24">
+        <v>45513.708333333336</v>
+      </c>
+      <c r="B72">
+        <v>6.0211600000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="24">
+        <v>45513.958333333336</v>
+      </c>
+      <c r="B73">
+        <v>6.0135500000000004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="24">
+        <v>45514.458333333336</v>
+      </c>
+      <c r="B74">
+        <v>6.0135500000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="24">
+        <v>45514.708333333336</v>
+      </c>
+      <c r="B75">
+        <v>6.0135500000000004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="24">
+        <v>45514.958333333336</v>
+      </c>
+      <c r="B76">
+        <v>6.0135500000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="24">
+        <v>45515.458333333336</v>
+      </c>
+      <c r="B77">
+        <v>6.0078100000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="24">
+        <v>45515.708333333336</v>
+      </c>
+      <c r="B78">
+        <v>6.0093300000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="24">
+        <v>45515.958333333336</v>
+      </c>
+      <c r="B79">
+        <v>6.0075200000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="24">
+        <v>45516.458333333336</v>
+      </c>
+      <c r="B80">
+        <v>6.0078100000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="24">
+        <v>45516.708333333336</v>
+      </c>
+      <c r="B81">
+        <v>6.0093300000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="24">
+        <v>45516.958333333336</v>
+      </c>
+      <c r="B82">
+        <v>6.0075200000000004</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="24">
+        <v>45517.458333333336</v>
+      </c>
+      <c r="B83">
+        <v>6.0146800000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="24">
+        <v>45517.458333333336</v>
+      </c>
+      <c r="B84">
+        <v>5.9917600000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="24">
+        <v>45517.708333333336</v>
+      </c>
+      <c r="B85">
+        <v>5.9986600000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="24">
+        <v>45518.958333333336</v>
+      </c>
+      <c r="B86">
+        <v>6.0144599999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="24">
+        <v>45518.458333333336</v>
+      </c>
+      <c r="B87">
+        <v>6.0229699999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="24">
+        <v>45518.458333333336</v>
+      </c>
+      <c r="B88">
+        <v>6.0214800000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="24">
+        <v>45519.708333333336</v>
+      </c>
+      <c r="B89">
+        <v>5.9838699999999996</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="24">
+        <v>45519.958333333336</v>
+      </c>
+      <c r="B90">
+        <v>6.0173199999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="24">
+        <v>45519.458333333336</v>
+      </c>
+      <c r="B91">
+        <v>6.0248200000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="24">
+        <v>45520.708333333336</v>
+      </c>
+      <c r="B92">
+        <v>6.0010300000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="24">
+        <v>45520.958333333336</v>
+      </c>
+      <c r="B93">
+        <v>6.0262700000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="24">
+        <v>45520.458333333336</v>
+      </c>
+      <c r="B94">
+        <v>6.03376</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="24">
+        <v>45521.708333333336</v>
+      </c>
+      <c r="B95">
+        <v>6.03376</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="24">
+        <v>45521.958333333336</v>
+      </c>
+      <c r="B96">
+        <v>6.03376</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="24">
+        <v>45521.458333333336</v>
+      </c>
+      <c r="B97">
+        <v>6.03376</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="24">
+        <v>45522.708333333336</v>
+      </c>
+      <c r="B98">
+        <v>6.03376</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="24">
+        <v>45522.958333333336</v>
+      </c>
+      <c r="B99">
+        <v>6.03376</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="24">
+        <v>45522.458333333336</v>
+      </c>
+      <c r="B100">
+        <v>6.0332999999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="24">
+        <v>45523.458333333336</v>
+      </c>
+      <c r="B101">
+        <v>5.9958999999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="24">
+        <v>45523.708333333336</v>
+      </c>
+      <c r="B102">
+        <v>5.9989999999999997</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="24">
+        <v>45523.958333333336</v>
+      </c>
+      <c r="B103">
+        <v>5.9932999999999996</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="24">
+        <v>45524.458333333336</v>
+      </c>
+      <c r="B104">
+        <v>6.0391000000000004</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="24">
+        <v>45524.708333333336</v>
+      </c>
+      <c r="B105">
+        <v>6.1021000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="24">
+        <v>45524.958333333336</v>
+      </c>
+      <c r="B106">
+        <v>6.0941000000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="24">
+        <v>45525.458333333336</v>
+      </c>
+      <c r="B107">
+        <v>6.0796000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="24">
+        <v>45525.708333333336</v>
+      </c>
+      <c r="B108">
+        <v>6.1125999999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="24">
+        <v>45525.958333333336</v>
+      </c>
+      <c r="B109">
+        <v>6.1108000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="24">
+        <v>45526.458333333336</v>
+      </c>
+      <c r="B110">
+        <v>6.1086999999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="24">
+        <v>45526.708333333336</v>
+      </c>
+      <c r="B111">
+        <v>6.2092999999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="24">
+        <v>45526.958333333336</v>
+      </c>
+      <c r="B112">
+        <v>6.2225999999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="24">
+        <v>45527.458333333336</v>
+      </c>
+      <c r="B113">
+        <v>6.1725000000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="24">
+        <v>45527.708333333336</v>
+      </c>
+      <c r="B114">
+        <v>6.1323999999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="24">
+        <v>45527.958333333336</v>
+      </c>
+      <c r="B115">
+        <v>6.1401700000000003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="24">
+        <v>45528.458333333336</v>
+      </c>
+      <c r="B116">
+        <v>6.1401700000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="24">
+        <v>45528.458333333336</v>
+      </c>
+      <c r="B117">
+        <v>6.1401700000000003</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="24">
+        <v>45528.708333333336</v>
+      </c>
+      <c r="B118">
+        <v>6.1401700000000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="24">
+        <v>45529.958333333336</v>
+      </c>
+      <c r="B119">
+        <v>6.1401700000000003</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="24">
+        <v>45529.458333333336</v>
+      </c>
+      <c r="B120">
+        <v>6.1401700000000003</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="24">
+        <v>45529.708333333336</v>
+      </c>
+      <c r="B121">
+        <v>6.1395999999999997</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="24">
+        <v>45530.458333333336</v>
+      </c>
+      <c r="B122">
+        <v>6.1208999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="24">
+        <v>45530.708333333336</v>
+      </c>
+      <c r="B123">
+        <v>6.1284999999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="24">
+        <v>45530.958333333336</v>
+      </c>
+      <c r="B124">
+        <v>6.1401000000000003</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="24">
+        <v>45531.458333333336</v>
+      </c>
+      <c r="B125">
+        <v>6.1345000000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="24">
+        <v>45531.708333333336</v>
+      </c>
+      <c r="B126">
+        <v>6.1538000000000004</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="24">
+        <v>45531.958333333336</v>
+      </c>
+      <c r="B127">
+        <v>6.1562000000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="24">
+        <v>45532.458333333336</v>
+      </c>
+      <c r="B128">
+        <v>6.1444999999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="24">
+        <v>45532.708333333336</v>
+      </c>
+      <c r="B129">
+        <v>6.1733000000000002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="24">
+        <v>45532.958333333336</v>
+      </c>
+      <c r="B130">
+        <v>6.1912000000000003</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="24">
+        <v>45533.458333333336</v>
+      </c>
+      <c r="B131">
+        <v>6.2511999999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="24">
+        <v>45533.708333333336</v>
+      </c>
+      <c r="B132">
+        <v>6.2274000000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="24">
+        <v>45533.958333333336</v>
+      </c>
+      <c r="B133">
+        <v>6.2314999999999996</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="24">
+        <v>45534.458333333336</v>
+      </c>
+      <c r="B134">
+        <v>6.2614000000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="24">
+        <v>45534.708333333336</v>
+      </c>
+      <c r="B135">
+        <v>6.2282000000000002</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="24">
+        <v>45534.958333333336</v>
+      </c>
+      <c r="B136">
+        <v>6.1933699999999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="24">
+        <v>45535.458333333336</v>
+      </c>
+      <c r="B137">
+        <v>6.1933699999999998</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="24">
+        <v>45535.708333333336</v>
+      </c>
+      <c r="B138">
+        <v>6.1933699999999998</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="24">
+        <v>45535.958333333336</v>
+      </c>
+      <c r="B139">
+        <v>6.1933699999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="24">
+        <v>45536.458333333336</v>
+      </c>
+      <c r="B140">
+        <v>6.1933699999999998</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="24">
+        <v>45536.708333333336</v>
+      </c>
+      <c r="B141">
+        <v>6.1933699999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="24">
+        <v>45536.958333333336</v>
+      </c>
+      <c r="B142">
+        <v>6.2034399999999996</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="24">
+        <v>45537.458333333336</v>
+      </c>
+      <c r="B143">
+        <v>6.2514799999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="24">
+        <v>45537.708333333336</v>
+      </c>
+      <c r="B144">
+        <v>6.2182700000000004</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="24">
+        <v>45537.958333333336</v>
+      </c>
+      <c r="B145">
+        <v>6.2155399999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="24">
+        <v>45538.458333333336</v>
+      </c>
+      <c r="B146">
+        <v>6.2251500000000002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="24">
+        <v>45538.708333333336</v>
+      </c>
+      <c r="B147">
+        <v>6.2280600000000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="24">
+        <v>45538.958333333336</v>
+      </c>
+      <c r="B148">
+        <v>6.2437500000000004</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="24">
+        <v>45539.458333333336</v>
+      </c>
+      <c r="B149">
+        <v>6.2382799999999996</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="24">
+        <v>45539.708333333336</v>
+      </c>
+      <c r="B150">
+        <v>6.2497699999999998</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="24">
+        <v>45539.958333333336</v>
+      </c>
+      <c r="B151">
+        <v>6.2532800000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="24">
+        <v>45540.458333333336</v>
+      </c>
+      <c r="B152">
+        <v>6.22342</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="24">
+        <v>45540.708333333336</v>
+      </c>
+      <c r="B153">
+        <v>6.1868999999999996</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="24">
+        <v>45540.958333333336</v>
+      </c>
+      <c r="B154">
+        <v>6.1872999999999996</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="24">
+        <v>45541.458333333336</v>
+      </c>
+      <c r="B155">
+        <v>6.1641300000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="24">
+        <v>45541.708333333336</v>
+      </c>
+      <c r="B156">
+        <v>6.1978099999999996</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="24">
+        <v>45541.958333333336</v>
+      </c>
+      <c r="B157">
+        <v>6.2072099999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="24">
+        <v>45542.458333333336</v>
+      </c>
+      <c r="B158">
+        <v>6.2072099999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="24">
+        <v>45542.708333333336</v>
+      </c>
+      <c r="B159">
+        <v>6.2072099999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="24">
+        <v>45542.958333333336</v>
+      </c>
+      <c r="B160">
+        <v>6.2072099999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="24">
+        <v>45543.458333333336</v>
+      </c>
+      <c r="B161">
+        <v>6.2072099999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="24">
+        <v>45543.708333333336</v>
+      </c>
+      <c r="B162">
+        <v>6.2072099999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="24">
+        <v>45543.958333333336</v>
+      </c>
+      <c r="B163">
+        <v>6.2043600000000003</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="24">
+        <v>45544.458333333336</v>
+      </c>
+      <c r="B164">
+        <v>6.1954399999999996</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="24">
+        <v>45544.708333333336</v>
+      </c>
+      <c r="B165">
+        <v>6.1645099999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="24">
+        <v>45544.958333333336</v>
+      </c>
+      <c r="B166">
+        <v>6.1646200000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="24">
+        <v>45545.458333333336</v>
+      </c>
+      <c r="B167">
+        <v>6.1889099999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="24">
+        <v>45545.708333333336</v>
+      </c>
+      <c r="B168">
+        <v>6.2345699999999997</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="24">
+        <v>45545.958333333336</v>
+      </c>
+      <c r="B169">
+        <v>6.2496900000000002</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="24">
+        <v>45546.458333333336</v>
+      </c>
+      <c r="B170">
+        <v>6.2134999999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="24">
+        <v>45546.708333333336</v>
+      </c>
+      <c r="B171">
+        <v>6.2330899999999998</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="24">
+        <v>45546.958333333336</v>
+      </c>
+      <c r="B172">
+        <v>6.2430500000000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="24">
+        <v>45547.458333333336</v>
+      </c>
+      <c r="B173">
+        <v>6.2440899999999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="24">
+        <v>45547.708333333336</v>
+      </c>
+      <c r="B174">
+        <v>6.2191299999999998</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="24">
+        <v>45547.958333333336</v>
+      </c>
+      <c r="B175">
+        <v>6.2359799999999996</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="24">
+        <v>45548.458333333336</v>
+      </c>
+      <c r="B176">
+        <v>6.1826600000000003</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="24">
+        <v>45548.708333333336</v>
+      </c>
+      <c r="B177">
+        <v>6.1648899999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="24">
+        <v>45548.958333333336</v>
+      </c>
+      <c r="B178">
+        <v>6.1635600000000004</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="24">
+        <v>45549.458333333336</v>
+      </c>
+      <c r="B179">
+        <v>6.1635600000000004</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="24">
+        <v>45549.708333333336</v>
+      </c>
+      <c r="B180">
+        <v>6.1635600000000004</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="24">
+        <v>45549.958333333336</v>
+      </c>
+      <c r="B181">
+        <v>6.1635600000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E2342F-700D-4437-99A3-C35FCA707D45}">
   <dimension ref="A1:C33"/>
   <sheetViews>
@@ -13597,12 +16537,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="20">
         <f>AVERAGE('2024_wise_usd'!$K3:$K55)</f>
@@ -13615,7 +16555,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="20">
         <f>_xlfn.STDEV.S('2024_wise_usd'!$K3:$K55)</f>
@@ -13628,7 +16568,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="20">
         <f>AVERAGE('2024_wise_usd'!$J3:$J55)</f>
@@ -13641,7 +16581,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="20">
         <f>_xlfn.STDEV.S('2024_wise_usd'!$J3:$J55)</f>
@@ -13654,7 +16594,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="19">
         <f>B4*SQRT(360)</f>
@@ -13667,7 +16607,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="19">
         <f>B4*SQRT(252)</f>
@@ -13680,7 +16620,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="19">
         <f>B6*SQRT(360)</f>
@@ -13693,7 +16633,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="19">
         <f>B6*SQRT(252)</f>
@@ -13706,12 +16646,12 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="20">
         <f>AVERAGE('2024_wise_eur'!$K3:$K55)</f>
@@ -13724,7 +16664,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="20">
         <f>_xlfn.STDEV.S('2024_wise_eur'!$K3:$K55)</f>
@@ -13737,7 +16677,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="20">
         <f>AVERAGE('2024_wise_eur'!$J3:$J55)</f>
@@ -13750,7 +16690,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="20">
         <f>_xlfn.STDEV.S('2024_wise_eur'!$J3:$J55)</f>
@@ -13763,7 +16703,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="19">
         <f>B17*SQRT(360)</f>
@@ -13776,7 +16716,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="19">
         <f>B17*SQRT(252)</f>
@@ -13789,7 +16729,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="19">
         <f>B19*SQRT(360)</f>
@@ -13802,7 +16742,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="19">
         <f>B19*SQRT(252)</f>
@@ -13815,12 +16755,12 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29">
         <v>20</v>
@@ -13828,7 +16768,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -13836,7 +16776,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -13844,7 +16784,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="23">
         <f>$B$31/(1+B29)</f>
@@ -13853,7 +16793,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="23">
         <f>$B$31/(1+B30)</f>

</xml_diff>